<commit_message>
Add unit tests for adx_ingest_function, utils.py & excel_generator
</commit_message>
<xml_diff>
--- a/backend/data_engineering/FormattedAnnualBudget.xlsx
+++ b/backend/data_engineering/FormattedAnnualBudget.xlsx
@@ -1719,8 +1719,8 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D2:D5"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D2:D5"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="A6:A9"/>
@@ -2480,11 +2480,11 @@
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C4:C12"/>
     <mergeCell ref="A4:A12"/>
     <mergeCell ref="E15"/>
     <mergeCell ref="D13:D15"/>
-    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -2991,8 +2991,8 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="C4:C6"/>
   </mergeCells>
@@ -3006,7 +3006,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BN287"/>
+  <dimension ref="A1:BN256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3037,15 +3037,15 @@
     <col width="11" customWidth="1" min="21" max="21"/>
     <col width="13" customWidth="1" min="22" max="22"/>
     <col width="18" customWidth="1" min="23" max="23"/>
-    <col width="19" customWidth="1" min="24" max="24"/>
+    <col width="11" customWidth="1" min="24" max="24"/>
     <col width="17" customWidth="1" min="25" max="25"/>
     <col width="11" customWidth="1" min="26" max="26"/>
     <col width="13" customWidth="1" min="27" max="27"/>
     <col width="19" customWidth="1" min="28" max="28"/>
-    <col width="19" customWidth="1" min="29" max="29"/>
+    <col width="11" customWidth="1" min="29" max="29"/>
     <col width="17" customWidth="1" min="30" max="30"/>
     <col width="11" customWidth="1" min="31" max="31"/>
-    <col width="19" customWidth="1" min="32" max="32"/>
+    <col width="13" customWidth="1" min="32" max="32"/>
     <col width="19" customWidth="1" min="33" max="33"/>
     <col width="19" customWidth="1" min="34" max="34"/>
     <col width="19" customWidth="1" min="35" max="35"/>
@@ -26780,2562 +26780,6 @@
       <c r="BM256" s="11" t="n"/>
       <c r="BN256" s="11" t="n"/>
     </row>
-    <row r="257">
-      <c r="A257" s="2" t="n"/>
-      <c r="B257" s="5" t="n"/>
-      <c r="C257" s="5" t="n"/>
-      <c r="D257" s="6" t="n"/>
-      <c r="E257" s="2" t="n"/>
-      <c r="F257" s="7" t="n"/>
-      <c r="G257" s="8" t="n"/>
-      <c r="H257" s="8" t="n"/>
-      <c r="I257" s="8" t="n"/>
-      <c r="J257" s="2" t="n"/>
-      <c r="K257" s="2" t="n"/>
-      <c r="L257" s="8" t="n"/>
-      <c r="M257" s="8" t="n"/>
-      <c r="N257" s="8" t="n"/>
-      <c r="O257" s="2" t="n"/>
-      <c r="P257" s="2" t="n"/>
-      <c r="Q257" s="8" t="n"/>
-      <c r="R257" s="8" t="n"/>
-      <c r="S257" s="8" t="n"/>
-      <c r="T257" s="2" t="n"/>
-      <c r="U257" s="2" t="n"/>
-      <c r="V257" s="8" t="n"/>
-      <c r="W257" s="8" t="n">
-        <v>2000</v>
-      </c>
-      <c r="X257" s="8" t="n">
-        <v>70</v>
-      </c>
-      <c r="Y257" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="Z257" s="2" t="n">
-        <v>2090</v>
-      </c>
-      <c r="AA257" s="8" t="n">
-        <v>3450</v>
-      </c>
-      <c r="AB257" s="8" t="n">
-        <v>120.75</v>
-      </c>
-      <c r="AC257" s="8" t="n">
-        <v>34.5</v>
-      </c>
-      <c r="AD257" s="2" t="n">
-        <v>3605.25</v>
-      </c>
-      <c r="AE257" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="AF257" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="AG257" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH257" s="8" t="n">
-        <v>208</v>
-      </c>
-      <c r="AI257" s="2" t="n"/>
-      <c r="AJ257" s="2" t="n"/>
-      <c r="AK257" s="8" t="n"/>
-      <c r="AL257" s="8" t="n"/>
-      <c r="AM257" s="8" t="n"/>
-      <c r="AN257" s="2" t="n"/>
-      <c r="AO257" s="2" t="n"/>
-      <c r="AP257" s="8" t="n"/>
-      <c r="AQ257" s="8" t="n"/>
-      <c r="AR257" s="8" t="n"/>
-      <c r="AS257" s="2" t="n"/>
-      <c r="AT257" s="2" t="n"/>
-      <c r="AU257" s="8" t="n"/>
-      <c r="AV257" s="8" t="n"/>
-      <c r="AW257" s="8" t="n"/>
-      <c r="AX257" s="2" t="n"/>
-      <c r="AY257" s="2" t="n"/>
-      <c r="AZ257" s="8" t="n"/>
-      <c r="BA257" s="8" t="n"/>
-      <c r="BB257" s="8" t="n"/>
-      <c r="BC257" s="2" t="n"/>
-      <c r="BD257" s="2" t="n"/>
-      <c r="BE257" s="8" t="n"/>
-      <c r="BF257" s="8" t="n"/>
-      <c r="BG257" s="8" t="n"/>
-      <c r="BH257" s="2" t="n"/>
-      <c r="BI257" s="2" t="n"/>
-      <c r="BJ257" s="8" t="n"/>
-      <c r="BK257" s="8" t="n"/>
-      <c r="BL257" s="8" t="n"/>
-      <c r="BM257" s="2" t="n"/>
-      <c r="BN257" s="2" t="n"/>
-    </row>
-    <row r="258">
-      <c r="A258" s="2" t="n"/>
-      <c r="B258" s="5" t="n"/>
-      <c r="C258" s="5" t="n"/>
-      <c r="D258" s="6" t="n"/>
-      <c r="E258" s="2" t="n"/>
-      <c r="F258" s="7" t="n"/>
-      <c r="G258" s="8" t="n"/>
-      <c r="H258" s="8" t="n"/>
-      <c r="I258" s="8" t="n"/>
-      <c r="J258" s="2" t="n"/>
-      <c r="K258" s="2" t="n"/>
-      <c r="L258" s="8" t="n"/>
-      <c r="M258" s="8" t="n"/>
-      <c r="N258" s="8" t="n"/>
-      <c r="O258" s="2" t="n"/>
-      <c r="P258" s="2" t="n"/>
-      <c r="Q258" s="8" t="n"/>
-      <c r="R258" s="8" t="n"/>
-      <c r="S258" s="8" t="n"/>
-      <c r="T258" s="2" t="n"/>
-      <c r="U258" s="2" t="n"/>
-      <c r="V258" s="8" t="n"/>
-      <c r="W258" s="8" t="n">
-        <v>2300</v>
-      </c>
-      <c r="X258" s="8" t="n">
-        <v>80.50000000000001</v>
-      </c>
-      <c r="Y258" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="Z258" s="2" t="n">
-        <v>2403.5</v>
-      </c>
-      <c r="AA258" s="8" t="n">
-        <v>3445</v>
-      </c>
-      <c r="AB258" s="8" t="n">
-        <v>120.575</v>
-      </c>
-      <c r="AC258" s="8" t="n">
-        <v>34.45</v>
-      </c>
-      <c r="AD258" s="2" t="n">
-        <v>3600.025</v>
-      </c>
-      <c r="AE258" s="2" t="n">
-        <v>15350</v>
-      </c>
-      <c r="AF258" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG258" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH258" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI258" s="2" t="n"/>
-      <c r="AJ258" s="2" t="n"/>
-      <c r="AK258" s="8" t="n"/>
-      <c r="AL258" s="8" t="n"/>
-      <c r="AM258" s="8" t="n"/>
-      <c r="AN258" s="2" t="n"/>
-      <c r="AO258" s="2" t="n"/>
-      <c r="AP258" s="8" t="n"/>
-      <c r="AQ258" s="8" t="n"/>
-      <c r="AR258" s="8" t="n"/>
-      <c r="AS258" s="2" t="n"/>
-      <c r="AT258" s="2" t="n"/>
-      <c r="AU258" s="8" t="n"/>
-      <c r="AV258" s="8" t="n"/>
-      <c r="AW258" s="8" t="n"/>
-      <c r="AX258" s="2" t="n"/>
-      <c r="AY258" s="2" t="n"/>
-      <c r="AZ258" s="8" t="n"/>
-      <c r="BA258" s="8" t="n"/>
-      <c r="BB258" s="8" t="n"/>
-      <c r="BC258" s="2" t="n"/>
-      <c r="BD258" s="2" t="n"/>
-      <c r="BE258" s="8" t="n"/>
-      <c r="BF258" s="8" t="n"/>
-      <c r="BG258" s="8" t="n"/>
-      <c r="BH258" s="2" t="n"/>
-      <c r="BI258" s="2" t="n"/>
-      <c r="BJ258" s="8" t="n"/>
-      <c r="BK258" s="8" t="n"/>
-      <c r="BL258" s="8" t="n"/>
-      <c r="BM258" s="2" t="n"/>
-      <c r="BN258" s="2" t="n"/>
-    </row>
-    <row r="259">
-      <c r="A259" s="2" t="n"/>
-      <c r="B259" s="5" t="n"/>
-      <c r="C259" s="5" t="n"/>
-      <c r="D259" s="6" t="n"/>
-      <c r="E259" s="2" t="n"/>
-      <c r="F259" s="7" t="n"/>
-      <c r="G259" s="8" t="n"/>
-      <c r="H259" s="8" t="n"/>
-      <c r="I259" s="8" t="n"/>
-      <c r="J259" s="2" t="n"/>
-      <c r="K259" s="2" t="n"/>
-      <c r="L259" s="8" t="n"/>
-      <c r="M259" s="8" t="n"/>
-      <c r="N259" s="8" t="n"/>
-      <c r="O259" s="2" t="n"/>
-      <c r="P259" s="2" t="n"/>
-      <c r="Q259" s="8" t="n"/>
-      <c r="R259" s="8" t="n"/>
-      <c r="S259" s="8" t="n"/>
-      <c r="T259" s="2" t="n"/>
-      <c r="U259" s="2" t="n"/>
-      <c r="V259" s="8" t="n"/>
-      <c r="W259" s="8" t="n"/>
-      <c r="X259" s="8" t="n"/>
-      <c r="Y259" s="2" t="n"/>
-      <c r="Z259" s="2" t="n"/>
-      <c r="AA259" s="8" t="n">
-        <v>2650</v>
-      </c>
-      <c r="AB259" s="8" t="n">
-        <v>92.75</v>
-      </c>
-      <c r="AC259" s="8" t="n">
-        <v>26.5</v>
-      </c>
-      <c r="AD259" s="2" t="n">
-        <v>2769.25</v>
-      </c>
-      <c r="AE259" s="2" t="n">
-        <v>12930</v>
-      </c>
-      <c r="AF259" s="8" t="n">
-        <v>452.5500000000001</v>
-      </c>
-      <c r="AG259" s="8" t="n">
-        <v>129.3</v>
-      </c>
-      <c r="AH259" s="8" t="n">
-        <v>13511.85</v>
-      </c>
-      <c r="AI259" s="2" t="n"/>
-      <c r="AJ259" s="2" t="n"/>
-      <c r="AK259" s="8" t="n"/>
-      <c r="AL259" s="8" t="n"/>
-      <c r="AM259" s="8" t="n"/>
-      <c r="AN259" s="2" t="n"/>
-      <c r="AO259" s="2" t="n"/>
-      <c r="AP259" s="8" t="n"/>
-      <c r="AQ259" s="8" t="n"/>
-      <c r="AR259" s="8" t="n"/>
-      <c r="AS259" s="2" t="n"/>
-      <c r="AT259" s="2" t="n"/>
-      <c r="AU259" s="8" t="n"/>
-      <c r="AV259" s="8" t="n"/>
-      <c r="AW259" s="8" t="n"/>
-      <c r="AX259" s="2" t="n"/>
-      <c r="AY259" s="2" t="n"/>
-      <c r="AZ259" s="8" t="n"/>
-      <c r="BA259" s="8" t="n"/>
-      <c r="BB259" s="8" t="n"/>
-      <c r="BC259" s="2" t="n"/>
-      <c r="BD259" s="2" t="n"/>
-      <c r="BE259" s="8" t="n"/>
-      <c r="BF259" s="8" t="n"/>
-      <c r="BG259" s="8" t="n"/>
-      <c r="BH259" s="2" t="n"/>
-      <c r="BI259" s="2" t="n"/>
-      <c r="BJ259" s="8" t="n"/>
-      <c r="BK259" s="8" t="n"/>
-      <c r="BL259" s="8" t="n"/>
-      <c r="BM259" s="2" t="n"/>
-      <c r="BN259" s="2" t="n"/>
-    </row>
-    <row r="260">
-      <c r="A260" s="2" t="n"/>
-      <c r="B260" s="5" t="n"/>
-      <c r="C260" s="5" t="n"/>
-      <c r="D260" s="6" t="n"/>
-      <c r="E260" s="2" t="n"/>
-      <c r="F260" s="7" t="n"/>
-      <c r="G260" s="8" t="n"/>
-      <c r="H260" s="8" t="n"/>
-      <c r="I260" s="8" t="n"/>
-      <c r="J260" s="2" t="n"/>
-      <c r="K260" s="2" t="n"/>
-      <c r="L260" s="8" t="n"/>
-      <c r="M260" s="8" t="n"/>
-      <c r="N260" s="8" t="n"/>
-      <c r="O260" s="2" t="n"/>
-      <c r="P260" s="2" t="n"/>
-      <c r="Q260" s="8" t="n"/>
-      <c r="R260" s="8" t="n"/>
-      <c r="S260" s="8" t="n"/>
-      <c r="T260" s="2" t="n"/>
-      <c r="U260" s="2" t="n"/>
-      <c r="V260" s="8" t="n"/>
-      <c r="W260" s="8" t="n"/>
-      <c r="X260" s="8" t="n"/>
-      <c r="Y260" s="2" t="n"/>
-      <c r="Z260" s="2" t="n"/>
-      <c r="AA260" s="8" t="n">
-        <v>1230</v>
-      </c>
-      <c r="AB260" s="8" t="n">
-        <v>43.05</v>
-      </c>
-      <c r="AC260" s="8" t="n">
-        <v>12.3</v>
-      </c>
-      <c r="AD260" s="2" t="n">
-        <v>1285.35</v>
-      </c>
-      <c r="AE260" s="2" t="n">
-        <v>2200</v>
-      </c>
-      <c r="AF260" s="8" t="n">
-        <v>66</v>
-      </c>
-      <c r="AG260" s="8" t="n">
-        <v>22</v>
-      </c>
-      <c r="AH260" s="8" t="n">
-        <v>2288</v>
-      </c>
-      <c r="AI260" s="2" t="n"/>
-      <c r="AJ260" s="2" t="n"/>
-      <c r="AK260" s="8" t="n"/>
-      <c r="AL260" s="8" t="n"/>
-      <c r="AM260" s="8" t="n"/>
-      <c r="AN260" s="2" t="n"/>
-      <c r="AO260" s="2" t="n"/>
-      <c r="AP260" s="8" t="n"/>
-      <c r="AQ260" s="8" t="n"/>
-      <c r="AR260" s="8" t="n"/>
-      <c r="AS260" s="2" t="n"/>
-      <c r="AT260" s="2" t="n"/>
-      <c r="AU260" s="8" t="n"/>
-      <c r="AV260" s="8" t="n"/>
-      <c r="AW260" s="8" t="n"/>
-      <c r="AX260" s="2" t="n"/>
-      <c r="AY260" s="2" t="n"/>
-      <c r="AZ260" s="8" t="n"/>
-      <c r="BA260" s="8" t="n"/>
-      <c r="BB260" s="8" t="n"/>
-      <c r="BC260" s="2" t="n"/>
-      <c r="BD260" s="2" t="n"/>
-      <c r="BE260" s="8" t="n"/>
-      <c r="BF260" s="8" t="n"/>
-      <c r="BG260" s="8" t="n"/>
-      <c r="BH260" s="2" t="n"/>
-      <c r="BI260" s="2" t="n"/>
-      <c r="BJ260" s="8" t="n"/>
-      <c r="BK260" s="8" t="n"/>
-      <c r="BL260" s="8" t="n"/>
-      <c r="BM260" s="2" t="n"/>
-      <c r="BN260" s="2" t="n"/>
-    </row>
-    <row r="261">
-      <c r="A261" s="2" t="n"/>
-      <c r="B261" s="5" t="n"/>
-      <c r="C261" s="5" t="n"/>
-      <c r="D261" s="6" t="n"/>
-      <c r="E261" s="2" t="n"/>
-      <c r="F261" s="7" t="n"/>
-      <c r="G261" s="8" t="n"/>
-      <c r="H261" s="8" t="n"/>
-      <c r="I261" s="8" t="n"/>
-      <c r="J261" s="2" t="n"/>
-      <c r="K261" s="2" t="n"/>
-      <c r="L261" s="8" t="n"/>
-      <c r="M261" s="8" t="n"/>
-      <c r="N261" s="8" t="n"/>
-      <c r="O261" s="2" t="n"/>
-      <c r="P261" s="2" t="n"/>
-      <c r="Q261" s="8" t="n"/>
-      <c r="R261" s="8" t="n"/>
-      <c r="S261" s="8" t="n"/>
-      <c r="T261" s="2" t="n"/>
-      <c r="U261" s="2" t="n"/>
-      <c r="V261" s="8" t="n"/>
-      <c r="W261" s="8" t="n"/>
-      <c r="X261" s="8" t="n"/>
-      <c r="Y261" s="2" t="n"/>
-      <c r="Z261" s="2" t="n"/>
-      <c r="AA261" s="8" t="n">
-        <v>1305</v>
-      </c>
-      <c r="AB261" s="8" t="n">
-        <v>45.675</v>
-      </c>
-      <c r="AC261" s="8" t="n">
-        <v>13.05</v>
-      </c>
-      <c r="AD261" s="2" t="n">
-        <v>1363.725</v>
-      </c>
-      <c r="AE261" s="2" t="n">
-        <v>1020</v>
-      </c>
-      <c r="AF261" s="8" t="n">
-        <v>30.6</v>
-      </c>
-      <c r="AG261" s="8" t="n">
-        <v>10.2</v>
-      </c>
-      <c r="AH261" s="8" t="n">
-        <v>1060.8</v>
-      </c>
-      <c r="AI261" s="2" t="n"/>
-      <c r="AJ261" s="2" t="n"/>
-      <c r="AK261" s="8" t="n"/>
-      <c r="AL261" s="8" t="n"/>
-      <c r="AM261" s="8" t="n"/>
-      <c r="AN261" s="2" t="n"/>
-      <c r="AO261" s="2" t="n"/>
-      <c r="AP261" s="8" t="n"/>
-      <c r="AQ261" s="8" t="n"/>
-      <c r="AR261" s="8" t="n"/>
-      <c r="AS261" s="2" t="n"/>
-      <c r="AT261" s="2" t="n"/>
-      <c r="AU261" s="8" t="n"/>
-      <c r="AV261" s="8" t="n"/>
-      <c r="AW261" s="8" t="n"/>
-      <c r="AX261" s="2" t="n"/>
-      <c r="AY261" s="2" t="n"/>
-      <c r="AZ261" s="8" t="n"/>
-      <c r="BA261" s="8" t="n"/>
-      <c r="BB261" s="8" t="n"/>
-      <c r="BC261" s="2" t="n"/>
-      <c r="BD261" s="2" t="n"/>
-      <c r="BE261" s="8" t="n"/>
-      <c r="BF261" s="8" t="n"/>
-      <c r="BG261" s="8" t="n"/>
-      <c r="BH261" s="2" t="n"/>
-      <c r="BI261" s="2" t="n"/>
-      <c r="BJ261" s="8" t="n"/>
-      <c r="BK261" s="8" t="n"/>
-      <c r="BL261" s="8" t="n"/>
-      <c r="BM261" s="2" t="n"/>
-      <c r="BN261" s="2" t="n"/>
-    </row>
-    <row r="262">
-      <c r="A262" s="2" t="n"/>
-      <c r="B262" s="5" t="n"/>
-      <c r="C262" s="5" t="n"/>
-      <c r="D262" s="6" t="n"/>
-      <c r="E262" s="2" t="n"/>
-      <c r="F262" s="7" t="n"/>
-      <c r="G262" s="8" t="n"/>
-      <c r="H262" s="8" t="n"/>
-      <c r="I262" s="8" t="n"/>
-      <c r="J262" s="2" t="n"/>
-      <c r="K262" s="2" t="n"/>
-      <c r="L262" s="8" t="n"/>
-      <c r="M262" s="8" t="n"/>
-      <c r="N262" s="8" t="n"/>
-      <c r="O262" s="2" t="n"/>
-      <c r="P262" s="2" t="n"/>
-      <c r="Q262" s="8" t="n"/>
-      <c r="R262" s="8" t="n"/>
-      <c r="S262" s="8" t="n"/>
-      <c r="T262" s="2" t="n"/>
-      <c r="U262" s="2" t="n"/>
-      <c r="V262" s="8" t="n"/>
-      <c r="W262" s="8" t="n"/>
-      <c r="X262" s="8" t="n"/>
-      <c r="Y262" s="2" t="n"/>
-      <c r="Z262" s="2" t="n"/>
-      <c r="AA262" s="8" t="n">
-        <v>3750</v>
-      </c>
-      <c r="AB262" s="8" t="n">
-        <v>131.25</v>
-      </c>
-      <c r="AC262" s="8" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="AD262" s="2" t="n">
-        <v>3918.75</v>
-      </c>
-      <c r="AE262" s="2" t="n">
-        <v>670</v>
-      </c>
-      <c r="AF262" s="8" t="n">
-        <v>20.1</v>
-      </c>
-      <c r="AG262" s="8" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="AH262" s="8" t="n">
-        <v>696.8000000000001</v>
-      </c>
-      <c r="AI262" s="2" t="n"/>
-      <c r="AJ262" s="2" t="n"/>
-      <c r="AK262" s="8" t="n"/>
-      <c r="AL262" s="8" t="n"/>
-      <c r="AM262" s="8" t="n"/>
-      <c r="AN262" s="2" t="n"/>
-      <c r="AO262" s="2" t="n"/>
-      <c r="AP262" s="8" t="n"/>
-      <c r="AQ262" s="8" t="n"/>
-      <c r="AR262" s="8" t="n"/>
-      <c r="AS262" s="2" t="n"/>
-      <c r="AT262" s="2" t="n"/>
-      <c r="AU262" s="8" t="n"/>
-      <c r="AV262" s="8" t="n"/>
-      <c r="AW262" s="8" t="n"/>
-      <c r="AX262" s="2" t="n"/>
-      <c r="AY262" s="2" t="n"/>
-      <c r="AZ262" s="8" t="n"/>
-      <c r="BA262" s="8" t="n"/>
-      <c r="BB262" s="8" t="n"/>
-      <c r="BC262" s="2" t="n"/>
-      <c r="BD262" s="2" t="n"/>
-      <c r="BE262" s="8" t="n"/>
-      <c r="BF262" s="8" t="n"/>
-      <c r="BG262" s="8" t="n"/>
-      <c r="BH262" s="2" t="n"/>
-      <c r="BI262" s="2" t="n"/>
-      <c r="BJ262" s="8" t="n"/>
-      <c r="BK262" s="8" t="n"/>
-      <c r="BL262" s="8" t="n"/>
-      <c r="BM262" s="2" t="n"/>
-      <c r="BN262" s="2" t="n"/>
-    </row>
-    <row r="263">
-      <c r="A263" s="2" t="n"/>
-      <c r="B263" s="5" t="n"/>
-      <c r="C263" s="5" t="n"/>
-      <c r="D263" s="6" t="n"/>
-      <c r="E263" s="2" t="n"/>
-      <c r="F263" s="7" t="n"/>
-      <c r="G263" s="8" t="n"/>
-      <c r="H263" s="8" t="n"/>
-      <c r="I263" s="8" t="n"/>
-      <c r="J263" s="2" t="n"/>
-      <c r="K263" s="2" t="n"/>
-      <c r="L263" s="8" t="n"/>
-      <c r="M263" s="8" t="n"/>
-      <c r="N263" s="8" t="n"/>
-      <c r="O263" s="2" t="n"/>
-      <c r="P263" s="2" t="n"/>
-      <c r="Q263" s="8" t="n"/>
-      <c r="R263" s="8" t="n"/>
-      <c r="S263" s="8" t="n"/>
-      <c r="T263" s="2" t="n"/>
-      <c r="U263" s="2" t="n"/>
-      <c r="V263" s="8" t="n"/>
-      <c r="W263" s="8" t="n"/>
-      <c r="X263" s="8" t="n"/>
-      <c r="Y263" s="2" t="n"/>
-      <c r="Z263" s="2" t="n"/>
-      <c r="AA263" s="8" t="n">
-        <v>3090</v>
-      </c>
-      <c r="AB263" s="8" t="n">
-        <v>108.15</v>
-      </c>
-      <c r="AC263" s="8" t="n">
-        <v>30.9</v>
-      </c>
-      <c r="AD263" s="2" t="n">
-        <v>3229.05</v>
-      </c>
-      <c r="AE263" s="2" t="n">
-        <v>870</v>
-      </c>
-      <c r="AF263" s="8" t="n">
-        <v>26.1</v>
-      </c>
-      <c r="AG263" s="8" t="n">
-        <v>8.700000000000001</v>
-      </c>
-      <c r="AH263" s="8" t="n">
-        <v>904.8</v>
-      </c>
-      <c r="AI263" s="2" t="n"/>
-      <c r="AJ263" s="2" t="n"/>
-      <c r="AK263" s="8" t="n"/>
-      <c r="AL263" s="8" t="n"/>
-      <c r="AM263" s="8" t="n"/>
-      <c r="AN263" s="2" t="n"/>
-      <c r="AO263" s="2" t="n"/>
-      <c r="AP263" s="8" t="n"/>
-      <c r="AQ263" s="8" t="n"/>
-      <c r="AR263" s="8" t="n"/>
-      <c r="AS263" s="2" t="n"/>
-      <c r="AT263" s="2" t="n"/>
-      <c r="AU263" s="8" t="n"/>
-      <c r="AV263" s="8" t="n"/>
-      <c r="AW263" s="8" t="n"/>
-      <c r="AX263" s="2" t="n"/>
-      <c r="AY263" s="2" t="n"/>
-      <c r="AZ263" s="8" t="n"/>
-      <c r="BA263" s="8" t="n"/>
-      <c r="BB263" s="8" t="n"/>
-      <c r="BC263" s="2" t="n"/>
-      <c r="BD263" s="2" t="n"/>
-      <c r="BE263" s="8" t="n"/>
-      <c r="BF263" s="8" t="n"/>
-      <c r="BG263" s="8" t="n"/>
-      <c r="BH263" s="2" t="n"/>
-      <c r="BI263" s="2" t="n"/>
-      <c r="BJ263" s="8" t="n"/>
-      <c r="BK263" s="8" t="n"/>
-      <c r="BL263" s="8" t="n"/>
-      <c r="BM263" s="2" t="n"/>
-      <c r="BN263" s="2" t="n"/>
-    </row>
-    <row r="264">
-      <c r="A264" s="2" t="n"/>
-      <c r="B264" s="5" t="n"/>
-      <c r="C264" s="5" t="n"/>
-      <c r="D264" s="6" t="n"/>
-      <c r="E264" s="2" t="n"/>
-      <c r="F264" s="7" t="n"/>
-      <c r="G264" s="8" t="n"/>
-      <c r="H264" s="8" t="n"/>
-      <c r="I264" s="8" t="n"/>
-      <c r="J264" s="2" t="n"/>
-      <c r="K264" s="2" t="n"/>
-      <c r="L264" s="8" t="n"/>
-      <c r="M264" s="8" t="n"/>
-      <c r="N264" s="8" t="n"/>
-      <c r="O264" s="2" t="n"/>
-      <c r="P264" s="2" t="n"/>
-      <c r="Q264" s="8" t="n"/>
-      <c r="R264" s="8" t="n"/>
-      <c r="S264" s="8" t="n"/>
-      <c r="T264" s="2" t="n"/>
-      <c r="U264" s="2" t="n"/>
-      <c r="V264" s="8" t="n"/>
-      <c r="W264" s="8" t="n"/>
-      <c r="X264" s="8" t="n"/>
-      <c r="Y264" s="2" t="n"/>
-      <c r="Z264" s="2" t="n"/>
-      <c r="AA264" s="8" t="n">
-        <v>1050</v>
-      </c>
-      <c r="AB264" s="8" t="n">
-        <v>36.75</v>
-      </c>
-      <c r="AC264" s="8" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="AD264" s="2" t="n">
-        <v>1097.25</v>
-      </c>
-      <c r="AE264" s="2" t="n">
-        <v>3340</v>
-      </c>
-      <c r="AF264" s="8" t="n">
-        <v>100.2</v>
-      </c>
-      <c r="AG264" s="8" t="n">
-        <v>33.4</v>
-      </c>
-      <c r="AH264" s="8" t="n">
-        <v>3473.6</v>
-      </c>
-      <c r="AI264" s="2" t="n"/>
-      <c r="AJ264" s="2" t="n"/>
-      <c r="AK264" s="8" t="n"/>
-      <c r="AL264" s="8" t="n"/>
-      <c r="AM264" s="8" t="n"/>
-      <c r="AN264" s="2" t="n"/>
-      <c r="AO264" s="2" t="n"/>
-      <c r="AP264" s="8" t="n"/>
-      <c r="AQ264" s="8" t="n"/>
-      <c r="AR264" s="8" t="n"/>
-      <c r="AS264" s="2" t="n"/>
-      <c r="AT264" s="2" t="n"/>
-      <c r="AU264" s="8" t="n"/>
-      <c r="AV264" s="8" t="n"/>
-      <c r="AW264" s="8" t="n"/>
-      <c r="AX264" s="2" t="n"/>
-      <c r="AY264" s="2" t="n"/>
-      <c r="AZ264" s="8" t="n"/>
-      <c r="BA264" s="8" t="n"/>
-      <c r="BB264" s="8" t="n"/>
-      <c r="BC264" s="2" t="n"/>
-      <c r="BD264" s="2" t="n"/>
-      <c r="BE264" s="8" t="n"/>
-      <c r="BF264" s="8" t="n"/>
-      <c r="BG264" s="8" t="n"/>
-      <c r="BH264" s="2" t="n"/>
-      <c r="BI264" s="2" t="n"/>
-      <c r="BJ264" s="8" t="n"/>
-      <c r="BK264" s="8" t="n"/>
-      <c r="BL264" s="8" t="n"/>
-      <c r="BM264" s="2" t="n"/>
-      <c r="BN264" s="2" t="n"/>
-    </row>
-    <row r="265">
-      <c r="A265" s="2" t="n"/>
-      <c r="B265" s="5" t="n"/>
-      <c r="C265" s="5" t="n"/>
-      <c r="D265" s="6" t="n"/>
-      <c r="E265" s="2" t="n"/>
-      <c r="F265" s="7" t="n"/>
-      <c r="G265" s="8" t="n"/>
-      <c r="H265" s="8" t="n"/>
-      <c r="I265" s="8" t="n"/>
-      <c r="J265" s="2" t="n"/>
-      <c r="K265" s="2" t="n"/>
-      <c r="L265" s="8" t="n"/>
-      <c r="M265" s="8" t="n"/>
-      <c r="N265" s="8" t="n"/>
-      <c r="O265" s="2" t="n"/>
-      <c r="P265" s="2" t="n"/>
-      <c r="Q265" s="8" t="n"/>
-      <c r="R265" s="8" t="n"/>
-      <c r="S265" s="8" t="n"/>
-      <c r="T265" s="2" t="n"/>
-      <c r="U265" s="2" t="n"/>
-      <c r="V265" s="8" t="n"/>
-      <c r="W265" s="8" t="n"/>
-      <c r="X265" s="8" t="n"/>
-      <c r="Y265" s="2" t="n"/>
-      <c r="Z265" s="2" t="n"/>
-      <c r="AA265" s="8" t="n">
-        <v>1650</v>
-      </c>
-      <c r="AB265" s="8" t="n">
-        <v>57.75000000000001</v>
-      </c>
-      <c r="AC265" s="8" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="AD265" s="2" t="n">
-        <v>1724.25</v>
-      </c>
-      <c r="AE265" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="AF265" s="8" t="n">
-        <v>6.899999999999999</v>
-      </c>
-      <c r="AG265" s="8" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="AH265" s="8" t="n">
-        <v>239.2</v>
-      </c>
-      <c r="AI265" s="2" t="n"/>
-      <c r="AJ265" s="2" t="n"/>
-      <c r="AK265" s="8" t="n"/>
-      <c r="AL265" s="8" t="n"/>
-      <c r="AM265" s="8" t="n"/>
-      <c r="AN265" s="2" t="n"/>
-      <c r="AO265" s="2" t="n"/>
-      <c r="AP265" s="8" t="n"/>
-      <c r="AQ265" s="8" t="n"/>
-      <c r="AR265" s="8" t="n"/>
-      <c r="AS265" s="2" t="n"/>
-      <c r="AT265" s="2" t="n"/>
-      <c r="AU265" s="8" t="n"/>
-      <c r="AV265" s="8" t="n"/>
-      <c r="AW265" s="8" t="n"/>
-      <c r="AX265" s="2" t="n"/>
-      <c r="AY265" s="2" t="n"/>
-      <c r="AZ265" s="8" t="n"/>
-      <c r="BA265" s="8" t="n"/>
-      <c r="BB265" s="8" t="n"/>
-      <c r="BC265" s="2" t="n"/>
-      <c r="BD265" s="2" t="n"/>
-      <c r="BE265" s="8" t="n"/>
-      <c r="BF265" s="8" t="n"/>
-      <c r="BG265" s="8" t="n"/>
-      <c r="BH265" s="2" t="n"/>
-      <c r="BI265" s="2" t="n"/>
-      <c r="BJ265" s="8" t="n"/>
-      <c r="BK265" s="8" t="n"/>
-      <c r="BL265" s="8" t="n"/>
-      <c r="BM265" s="2" t="n"/>
-      <c r="BN265" s="2" t="n"/>
-    </row>
-    <row r="266">
-      <c r="A266" s="2" t="n"/>
-      <c r="B266" s="5" t="n"/>
-      <c r="C266" s="5" t="n"/>
-      <c r="D266" s="6" t="n"/>
-      <c r="E266" s="2" t="n"/>
-      <c r="F266" s="7" t="n"/>
-      <c r="G266" s="8" t="n"/>
-      <c r="H266" s="8" t="n"/>
-      <c r="I266" s="8" t="n"/>
-      <c r="J266" s="2" t="n"/>
-      <c r="K266" s="2" t="n"/>
-      <c r="L266" s="8" t="n"/>
-      <c r="M266" s="8" t="n"/>
-      <c r="N266" s="8" t="n"/>
-      <c r="O266" s="2" t="n"/>
-      <c r="P266" s="2" t="n"/>
-      <c r="Q266" s="8" t="n"/>
-      <c r="R266" s="8" t="n"/>
-      <c r="S266" s="8" t="n"/>
-      <c r="T266" s="2" t="n"/>
-      <c r="U266" s="2" t="n"/>
-      <c r="V266" s="8" t="n"/>
-      <c r="W266" s="8" t="n"/>
-      <c r="X266" s="8" t="n"/>
-      <c r="Y266" s="2" t="n"/>
-      <c r="Z266" s="2" t="n"/>
-      <c r="AA266" s="8" t="n">
-        <v>1870</v>
-      </c>
-      <c r="AB266" s="8" t="n">
-        <v>65.45</v>
-      </c>
-      <c r="AC266" s="8" t="n">
-        <v>18.7</v>
-      </c>
-      <c r="AD266" s="2" t="n">
-        <v>1954.15</v>
-      </c>
-      <c r="AE266" s="2" t="n">
-        <v>1220</v>
-      </c>
-      <c r="AF266" s="8" t="n">
-        <v>36.6</v>
-      </c>
-      <c r="AG266" s="8" t="n">
-        <v>12.2</v>
-      </c>
-      <c r="AH266" s="8" t="n">
-        <v>1268.8</v>
-      </c>
-      <c r="AI266" s="2" t="n"/>
-      <c r="AJ266" s="2" t="n"/>
-      <c r="AK266" s="8" t="n"/>
-      <c r="AL266" s="8" t="n"/>
-      <c r="AM266" s="8" t="n"/>
-      <c r="AN266" s="2" t="n"/>
-      <c r="AO266" s="2" t="n"/>
-      <c r="AP266" s="8" t="n"/>
-      <c r="AQ266" s="8" t="n"/>
-      <c r="AR266" s="8" t="n"/>
-      <c r="AS266" s="2" t="n"/>
-      <c r="AT266" s="2" t="n"/>
-      <c r="AU266" s="8" t="n"/>
-      <c r="AV266" s="8" t="n"/>
-      <c r="AW266" s="8" t="n"/>
-      <c r="AX266" s="2" t="n"/>
-      <c r="AY266" s="2" t="n"/>
-      <c r="AZ266" s="8" t="n"/>
-      <c r="BA266" s="8" t="n"/>
-      <c r="BB266" s="8" t="n"/>
-      <c r="BC266" s="2" t="n"/>
-      <c r="BD266" s="2" t="n"/>
-      <c r="BE266" s="8" t="n"/>
-      <c r="BF266" s="8" t="n"/>
-      <c r="BG266" s="8" t="n"/>
-      <c r="BH266" s="2" t="n"/>
-      <c r="BI266" s="2" t="n"/>
-      <c r="BJ266" s="8" t="n"/>
-      <c r="BK266" s="8" t="n"/>
-      <c r="BL266" s="8" t="n"/>
-      <c r="BM266" s="2" t="n"/>
-      <c r="BN266" s="2" t="n"/>
-    </row>
-    <row r="267">
-      <c r="A267" s="2" t="n"/>
-      <c r="B267" s="5" t="n"/>
-      <c r="C267" s="5" t="n"/>
-      <c r="D267" s="6" t="n"/>
-      <c r="E267" s="2" t="n"/>
-      <c r="F267" s="7" t="n"/>
-      <c r="G267" s="8" t="n"/>
-      <c r="H267" s="8" t="n"/>
-      <c r="I267" s="8" t="n"/>
-      <c r="J267" s="2" t="n"/>
-      <c r="K267" s="2" t="n"/>
-      <c r="L267" s="8" t="n"/>
-      <c r="M267" s="8" t="n"/>
-      <c r="N267" s="8" t="n"/>
-      <c r="O267" s="2" t="n"/>
-      <c r="P267" s="2" t="n"/>
-      <c r="Q267" s="8" t="n"/>
-      <c r="R267" s="8" t="n"/>
-      <c r="S267" s="8" t="n"/>
-      <c r="T267" s="2" t="n"/>
-      <c r="U267" s="2" t="n"/>
-      <c r="V267" s="8" t="n"/>
-      <c r="W267" s="8" t="n"/>
-      <c r="X267" s="8" t="n"/>
-      <c r="Y267" s="2" t="n"/>
-      <c r="Z267" s="2" t="n"/>
-      <c r="AA267" s="8" t="n">
-        <v>1540</v>
-      </c>
-      <c r="AB267" s="8" t="n">
-        <v>53.90000000000001</v>
-      </c>
-      <c r="AC267" s="8" t="n">
-        <v>15.4</v>
-      </c>
-      <c r="AD267" s="2" t="n">
-        <v>1609.3</v>
-      </c>
-      <c r="AE267" s="2" t="n">
-        <v>5800</v>
-      </c>
-      <c r="AF267" s="8" t="n">
-        <v>174</v>
-      </c>
-      <c r="AG267" s="8" t="n">
-        <v>58</v>
-      </c>
-      <c r="AH267" s="8" t="n">
-        <v>6032</v>
-      </c>
-      <c r="AI267" s="2" t="n"/>
-      <c r="AJ267" s="2" t="n"/>
-      <c r="AK267" s="8" t="n"/>
-      <c r="AL267" s="8" t="n"/>
-      <c r="AM267" s="8" t="n"/>
-      <c r="AN267" s="2" t="n"/>
-      <c r="AO267" s="2" t="n"/>
-      <c r="AP267" s="8" t="n"/>
-      <c r="AQ267" s="8" t="n"/>
-      <c r="AR267" s="8" t="n"/>
-      <c r="AS267" s="2" t="n"/>
-      <c r="AT267" s="2" t="n"/>
-      <c r="AU267" s="8" t="n"/>
-      <c r="AV267" s="8" t="n"/>
-      <c r="AW267" s="8" t="n"/>
-      <c r="AX267" s="2" t="n"/>
-      <c r="AY267" s="2" t="n"/>
-      <c r="AZ267" s="8" t="n"/>
-      <c r="BA267" s="8" t="n"/>
-      <c r="BB267" s="8" t="n"/>
-      <c r="BC267" s="2" t="n"/>
-      <c r="BD267" s="2" t="n"/>
-      <c r="BE267" s="8" t="n"/>
-      <c r="BF267" s="8" t="n"/>
-      <c r="BG267" s="8" t="n"/>
-      <c r="BH267" s="2" t="n"/>
-      <c r="BI267" s="2" t="n"/>
-      <c r="BJ267" s="8" t="n"/>
-      <c r="BK267" s="8" t="n"/>
-      <c r="BL267" s="8" t="n"/>
-      <c r="BM267" s="2" t="n"/>
-      <c r="BN267" s="2" t="n"/>
-    </row>
-    <row r="268">
-      <c r="A268" s="2" t="n"/>
-      <c r="B268" s="5" t="n"/>
-      <c r="C268" s="5" t="n"/>
-      <c r="D268" s="6" t="n"/>
-      <c r="E268" s="2" t="n"/>
-      <c r="F268" s="7" t="n"/>
-      <c r="G268" s="8" t="n"/>
-      <c r="H268" s="8" t="n"/>
-      <c r="I268" s="8" t="n"/>
-      <c r="J268" s="2" t="n"/>
-      <c r="K268" s="2" t="n"/>
-      <c r="L268" s="8" t="n"/>
-      <c r="M268" s="8" t="n"/>
-      <c r="N268" s="8" t="n"/>
-      <c r="O268" s="2" t="n"/>
-      <c r="P268" s="2" t="n"/>
-      <c r="Q268" s="8" t="n"/>
-      <c r="R268" s="8" t="n"/>
-      <c r="S268" s="8" t="n"/>
-      <c r="T268" s="2" t="n"/>
-      <c r="U268" s="2" t="n"/>
-      <c r="V268" s="8" t="n"/>
-      <c r="W268" s="8" t="n"/>
-      <c r="X268" s="8" t="n"/>
-      <c r="Y268" s="2" t="n"/>
-      <c r="Z268" s="2" t="n"/>
-      <c r="AA268" s="8" t="n">
-        <v>1070</v>
-      </c>
-      <c r="AB268" s="8" t="n">
-        <v>37.45</v>
-      </c>
-      <c r="AC268" s="8" t="n">
-        <v>10.7</v>
-      </c>
-      <c r="AD268" s="2" t="n">
-        <v>1118.15</v>
-      </c>
-      <c r="AE268" s="2" t="n">
-        <v>1225</v>
-      </c>
-      <c r="AF268" s="8" t="n">
-        <v>42.87500000000001</v>
-      </c>
-      <c r="AG268" s="8" t="n">
-        <v>12.25</v>
-      </c>
-      <c r="AH268" s="8" t="n">
-        <v>1280.125</v>
-      </c>
-      <c r="AI268" s="2" t="n"/>
-      <c r="AJ268" s="2" t="n"/>
-      <c r="AK268" s="8" t="n"/>
-      <c r="AL268" s="8" t="n"/>
-      <c r="AM268" s="8" t="n"/>
-      <c r="AN268" s="2" t="n"/>
-      <c r="AO268" s="2" t="n"/>
-      <c r="AP268" s="8" t="n"/>
-      <c r="AQ268" s="8" t="n"/>
-      <c r="AR268" s="8" t="n"/>
-      <c r="AS268" s="2" t="n"/>
-      <c r="AT268" s="2" t="n"/>
-      <c r="AU268" s="8" t="n"/>
-      <c r="AV268" s="8" t="n"/>
-      <c r="AW268" s="8" t="n"/>
-      <c r="AX268" s="2" t="n"/>
-      <c r="AY268" s="2" t="n"/>
-      <c r="AZ268" s="8" t="n"/>
-      <c r="BA268" s="8" t="n"/>
-      <c r="BB268" s="8" t="n"/>
-      <c r="BC268" s="2" t="n"/>
-      <c r="BD268" s="2" t="n"/>
-      <c r="BE268" s="8" t="n"/>
-      <c r="BF268" s="8" t="n"/>
-      <c r="BG268" s="8" t="n"/>
-      <c r="BH268" s="2" t="n"/>
-      <c r="BI268" s="2" t="n"/>
-      <c r="BJ268" s="8" t="n"/>
-      <c r="BK268" s="8" t="n"/>
-      <c r="BL268" s="8" t="n"/>
-      <c r="BM268" s="2" t="n"/>
-      <c r="BN268" s="2" t="n"/>
-    </row>
-    <row r="269">
-      <c r="A269" s="2" t="n"/>
-      <c r="B269" s="5" t="n"/>
-      <c r="C269" s="5" t="n"/>
-      <c r="D269" s="6" t="n"/>
-      <c r="E269" s="2" t="n"/>
-      <c r="F269" s="7" t="n"/>
-      <c r="G269" s="8" t="n"/>
-      <c r="H269" s="8" t="n"/>
-      <c r="I269" s="8" t="n"/>
-      <c r="J269" s="2" t="n"/>
-      <c r="K269" s="2" t="n"/>
-      <c r="L269" s="8" t="n"/>
-      <c r="M269" s="8" t="n"/>
-      <c r="N269" s="8" t="n"/>
-      <c r="O269" s="2" t="n"/>
-      <c r="P269" s="2" t="n"/>
-      <c r="Q269" s="8" t="n"/>
-      <c r="R269" s="8" t="n"/>
-      <c r="S269" s="8" t="n"/>
-      <c r="T269" s="2" t="n"/>
-      <c r="U269" s="2" t="n"/>
-      <c r="V269" s="8" t="n"/>
-      <c r="W269" s="8" t="n"/>
-      <c r="X269" s="8" t="n"/>
-      <c r="Y269" s="2" t="n"/>
-      <c r="Z269" s="2" t="n"/>
-      <c r="AA269" s="8" t="n">
-        <v>5430</v>
-      </c>
-      <c r="AB269" s="8" t="n">
-        <v>190.05</v>
-      </c>
-      <c r="AC269" s="8" t="n">
-        <v>54.3</v>
-      </c>
-      <c r="AD269" s="2" t="n">
-        <v>5674.35</v>
-      </c>
-      <c r="AE269" s="2" t="n">
-        <v>1580</v>
-      </c>
-      <c r="AF269" s="8" t="n">
-        <v>55.3</v>
-      </c>
-      <c r="AG269" s="8" t="n">
-        <v>15.8</v>
-      </c>
-      <c r="AH269" s="8" t="n">
-        <v>1651.1</v>
-      </c>
-      <c r="AI269" s="2" t="n"/>
-      <c r="AJ269" s="2" t="n"/>
-      <c r="AK269" s="8" t="n"/>
-      <c r="AL269" s="8" t="n"/>
-      <c r="AM269" s="8" t="n"/>
-      <c r="AN269" s="2" t="n"/>
-      <c r="AO269" s="2" t="n"/>
-      <c r="AP269" s="8" t="n"/>
-      <c r="AQ269" s="8" t="n"/>
-      <c r="AR269" s="8" t="n"/>
-      <c r="AS269" s="2" t="n"/>
-      <c r="AT269" s="2" t="n"/>
-      <c r="AU269" s="8" t="n"/>
-      <c r="AV269" s="8" t="n"/>
-      <c r="AW269" s="8" t="n"/>
-      <c r="AX269" s="2" t="n"/>
-      <c r="AY269" s="2" t="n"/>
-      <c r="AZ269" s="8" t="n"/>
-      <c r="BA269" s="8" t="n"/>
-      <c r="BB269" s="8" t="n"/>
-      <c r="BC269" s="2" t="n"/>
-      <c r="BD269" s="2" t="n"/>
-      <c r="BE269" s="8" t="n"/>
-      <c r="BF269" s="8" t="n"/>
-      <c r="BG269" s="8" t="n"/>
-      <c r="BH269" s="2" t="n"/>
-      <c r="BI269" s="2" t="n"/>
-      <c r="BJ269" s="8" t="n"/>
-      <c r="BK269" s="8" t="n"/>
-      <c r="BL269" s="8" t="n"/>
-      <c r="BM269" s="2" t="n"/>
-      <c r="BN269" s="2" t="n"/>
-    </row>
-    <row r="270">
-      <c r="A270" s="2" t="n"/>
-      <c r="B270" s="5" t="n"/>
-      <c r="C270" s="5" t="n"/>
-      <c r="D270" s="6" t="n"/>
-      <c r="E270" s="2" t="n"/>
-      <c r="F270" s="7" t="n"/>
-      <c r="G270" s="8" t="n"/>
-      <c r="H270" s="8" t="n"/>
-      <c r="I270" s="8" t="n"/>
-      <c r="J270" s="2" t="n"/>
-      <c r="K270" s="2" t="n"/>
-      <c r="L270" s="8" t="n"/>
-      <c r="M270" s="8" t="n"/>
-      <c r="N270" s="8" t="n"/>
-      <c r="O270" s="2" t="n"/>
-      <c r="P270" s="2" t="n"/>
-      <c r="Q270" s="8" t="n"/>
-      <c r="R270" s="8" t="n"/>
-      <c r="S270" s="8" t="n"/>
-      <c r="T270" s="2" t="n"/>
-      <c r="U270" s="2" t="n"/>
-      <c r="V270" s="8" t="n"/>
-      <c r="W270" s="8" t="n"/>
-      <c r="X270" s="8" t="n"/>
-      <c r="Y270" s="2" t="n"/>
-      <c r="Z270" s="2" t="n"/>
-      <c r="AA270" s="8" t="n">
-        <v>2390</v>
-      </c>
-      <c r="AB270" s="8" t="n">
-        <v>83.65000000000001</v>
-      </c>
-      <c r="AC270" s="8" t="n">
-        <v>23.9</v>
-      </c>
-      <c r="AD270" s="2" t="n">
-        <v>2497.55</v>
-      </c>
-      <c r="AE270" s="2" t="n">
-        <v>1120</v>
-      </c>
-      <c r="AF270" s="8" t="n">
-        <v>39.2</v>
-      </c>
-      <c r="AG270" s="8" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="AH270" s="8" t="n">
-        <v>1170.4</v>
-      </c>
-      <c r="AI270" s="2" t="n"/>
-      <c r="AJ270" s="2" t="n"/>
-      <c r="AK270" s="8" t="n"/>
-      <c r="AL270" s="8" t="n"/>
-      <c r="AM270" s="8" t="n"/>
-      <c r="AN270" s="2" t="n"/>
-      <c r="AO270" s="2" t="n"/>
-      <c r="AP270" s="8" t="n"/>
-      <c r="AQ270" s="8" t="n"/>
-      <c r="AR270" s="8" t="n"/>
-      <c r="AS270" s="2" t="n"/>
-      <c r="AT270" s="2" t="n"/>
-      <c r="AU270" s="8" t="n"/>
-      <c r="AV270" s="8" t="n"/>
-      <c r="AW270" s="8" t="n"/>
-      <c r="AX270" s="2" t="n"/>
-      <c r="AY270" s="2" t="n"/>
-      <c r="AZ270" s="8" t="n"/>
-      <c r="BA270" s="8" t="n"/>
-      <c r="BB270" s="8" t="n"/>
-      <c r="BC270" s="2" t="n"/>
-      <c r="BD270" s="2" t="n"/>
-      <c r="BE270" s="8" t="n"/>
-      <c r="BF270" s="8" t="n"/>
-      <c r="BG270" s="8" t="n"/>
-      <c r="BH270" s="2" t="n"/>
-      <c r="BI270" s="2" t="n"/>
-      <c r="BJ270" s="8" t="n"/>
-      <c r="BK270" s="8" t="n"/>
-      <c r="BL270" s="8" t="n"/>
-      <c r="BM270" s="2" t="n"/>
-      <c r="BN270" s="2" t="n"/>
-    </row>
-    <row r="271">
-      <c r="A271" s="2" t="n"/>
-      <c r="B271" s="5" t="n"/>
-      <c r="C271" s="5" t="n"/>
-      <c r="D271" s="6" t="n"/>
-      <c r="E271" s="2" t="n"/>
-      <c r="F271" s="7" t="n"/>
-      <c r="G271" s="8" t="n"/>
-      <c r="H271" s="8" t="n"/>
-      <c r="I271" s="8" t="n"/>
-      <c r="J271" s="2" t="n"/>
-      <c r="K271" s="2" t="n"/>
-      <c r="L271" s="8" t="n"/>
-      <c r="M271" s="8" t="n"/>
-      <c r="N271" s="8" t="n"/>
-      <c r="O271" s="2" t="n"/>
-      <c r="P271" s="2" t="n"/>
-      <c r="Q271" s="8" t="n"/>
-      <c r="R271" s="8" t="n"/>
-      <c r="S271" s="8" t="n"/>
-      <c r="T271" s="2" t="n"/>
-      <c r="U271" s="2" t="n"/>
-      <c r="V271" s="8" t="n"/>
-      <c r="W271" s="8" t="n"/>
-      <c r="X271" s="8" t="n"/>
-      <c r="Y271" s="2" t="n"/>
-      <c r="Z271" s="2" t="n"/>
-      <c r="AA271" s="8" t="n">
-        <v>1050</v>
-      </c>
-      <c r="AB271" s="8" t="n">
-        <v>36.75</v>
-      </c>
-      <c r="AC271" s="8" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="AD271" s="2" t="n">
-        <v>1097.25</v>
-      </c>
-      <c r="AE271" s="2" t="n">
-        <v>1950</v>
-      </c>
-      <c r="AF271" s="8" t="n">
-        <v>68.25</v>
-      </c>
-      <c r="AG271" s="8" t="n">
-        <v>19.5</v>
-      </c>
-      <c r="AH271" s="8" t="n">
-        <v>2037.75</v>
-      </c>
-      <c r="AI271" s="2" t="n"/>
-      <c r="AJ271" s="2" t="n"/>
-      <c r="AK271" s="8" t="n"/>
-      <c r="AL271" s="8" t="n"/>
-      <c r="AM271" s="8" t="n"/>
-      <c r="AN271" s="2" t="n"/>
-      <c r="AO271" s="2" t="n"/>
-      <c r="AP271" s="8" t="n"/>
-      <c r="AQ271" s="8" t="n"/>
-      <c r="AR271" s="8" t="n"/>
-      <c r="AS271" s="2" t="n"/>
-      <c r="AT271" s="2" t="n"/>
-      <c r="AU271" s="8" t="n"/>
-      <c r="AV271" s="8" t="n"/>
-      <c r="AW271" s="8" t="n"/>
-      <c r="AX271" s="2" t="n"/>
-      <c r="AY271" s="2" t="n"/>
-      <c r="AZ271" s="8" t="n"/>
-      <c r="BA271" s="8" t="n"/>
-      <c r="BB271" s="8" t="n"/>
-      <c r="BC271" s="2" t="n"/>
-      <c r="BD271" s="2" t="n"/>
-      <c r="BE271" s="8" t="n"/>
-      <c r="BF271" s="8" t="n"/>
-      <c r="BG271" s="8" t="n"/>
-      <c r="BH271" s="2" t="n"/>
-      <c r="BI271" s="2" t="n"/>
-      <c r="BJ271" s="8" t="n"/>
-      <c r="BK271" s="8" t="n"/>
-      <c r="BL271" s="8" t="n"/>
-      <c r="BM271" s="2" t="n"/>
-      <c r="BN271" s="2" t="n"/>
-    </row>
-    <row r="272">
-      <c r="A272" s="2" t="n"/>
-      <c r="B272" s="5" t="n"/>
-      <c r="C272" s="5" t="n"/>
-      <c r="D272" s="6" t="n"/>
-      <c r="E272" s="2" t="n"/>
-      <c r="F272" s="7" t="n"/>
-      <c r="G272" s="8" t="n"/>
-      <c r="H272" s="8" t="n"/>
-      <c r="I272" s="8" t="n"/>
-      <c r="J272" s="2" t="n"/>
-      <c r="K272" s="2" t="n"/>
-      <c r="L272" s="8" t="n"/>
-      <c r="M272" s="8" t="n"/>
-      <c r="N272" s="8" t="n"/>
-      <c r="O272" s="2" t="n"/>
-      <c r="P272" s="2" t="n"/>
-      <c r="Q272" s="8" t="n"/>
-      <c r="R272" s="8" t="n"/>
-      <c r="S272" s="8" t="n"/>
-      <c r="T272" s="2" t="n"/>
-      <c r="U272" s="2" t="n"/>
-      <c r="V272" s="8" t="n"/>
-      <c r="W272" s="8" t="n"/>
-      <c r="X272" s="8" t="n"/>
-      <c r="Y272" s="2" t="n"/>
-      <c r="Z272" s="2" t="n"/>
-      <c r="AA272" s="8" t="n">
-        <v>3270</v>
-      </c>
-      <c r="AB272" s="8" t="n">
-        <v>114.45</v>
-      </c>
-      <c r="AC272" s="8" t="n">
-        <v>32.7</v>
-      </c>
-      <c r="AD272" s="2" t="n">
-        <v>3417.15</v>
-      </c>
-      <c r="AE272" s="2" t="n">
-        <v>1830</v>
-      </c>
-      <c r="AF272" s="8" t="n">
-        <v>64.05000000000001</v>
-      </c>
-      <c r="AG272" s="8" t="n">
-        <v>18.3</v>
-      </c>
-      <c r="AH272" s="8" t="n">
-        <v>1912.35</v>
-      </c>
-      <c r="AI272" s="2" t="n"/>
-      <c r="AJ272" s="2" t="n"/>
-      <c r="AK272" s="8" t="n"/>
-      <c r="AL272" s="8" t="n"/>
-      <c r="AM272" s="8" t="n"/>
-      <c r="AN272" s="2" t="n"/>
-      <c r="AO272" s="2" t="n"/>
-      <c r="AP272" s="8" t="n"/>
-      <c r="AQ272" s="8" t="n"/>
-      <c r="AR272" s="8" t="n"/>
-      <c r="AS272" s="2" t="n"/>
-      <c r="AT272" s="2" t="n"/>
-      <c r="AU272" s="8" t="n"/>
-      <c r="AV272" s="8" t="n"/>
-      <c r="AW272" s="8" t="n"/>
-      <c r="AX272" s="2" t="n"/>
-      <c r="AY272" s="2" t="n"/>
-      <c r="AZ272" s="8" t="n"/>
-      <c r="BA272" s="8" t="n"/>
-      <c r="BB272" s="8" t="n"/>
-      <c r="BC272" s="2" t="n"/>
-      <c r="BD272" s="2" t="n"/>
-      <c r="BE272" s="8" t="n"/>
-      <c r="BF272" s="8" t="n"/>
-      <c r="BG272" s="8" t="n"/>
-      <c r="BH272" s="2" t="n"/>
-      <c r="BI272" s="2" t="n"/>
-      <c r="BJ272" s="8" t="n"/>
-      <c r="BK272" s="8" t="n"/>
-      <c r="BL272" s="8" t="n"/>
-      <c r="BM272" s="2" t="n"/>
-      <c r="BN272" s="2" t="n"/>
-    </row>
-    <row r="273">
-      <c r="A273" s="2" t="n"/>
-      <c r="B273" s="5" t="n"/>
-      <c r="C273" s="5" t="n"/>
-      <c r="D273" s="6" t="n"/>
-      <c r="E273" s="2" t="n"/>
-      <c r="F273" s="7" t="n"/>
-      <c r="G273" s="8" t="n"/>
-      <c r="H273" s="8" t="n"/>
-      <c r="I273" s="8" t="n"/>
-      <c r="J273" s="2" t="n"/>
-      <c r="K273" s="2" t="n"/>
-      <c r="L273" s="8" t="n"/>
-      <c r="M273" s="8" t="n"/>
-      <c r="N273" s="8" t="n"/>
-      <c r="O273" s="2" t="n"/>
-      <c r="P273" s="2" t="n"/>
-      <c r="Q273" s="8" t="n"/>
-      <c r="R273" s="8" t="n"/>
-      <c r="S273" s="8" t="n"/>
-      <c r="T273" s="2" t="n"/>
-      <c r="U273" s="2" t="n"/>
-      <c r="V273" s="8" t="n"/>
-      <c r="W273" s="8" t="n"/>
-      <c r="X273" s="8" t="n"/>
-      <c r="Y273" s="2" t="n"/>
-      <c r="Z273" s="2" t="n"/>
-      <c r="AA273" s="8" t="n">
-        <v>5600</v>
-      </c>
-      <c r="AB273" s="8" t="n">
-        <v>196</v>
-      </c>
-      <c r="AC273" s="8" t="n">
-        <v>56</v>
-      </c>
-      <c r="AD273" s="2" t="n">
-        <v>5852</v>
-      </c>
-      <c r="AE273" s="2" t="n">
-        <v>1275</v>
-      </c>
-      <c r="AF273" s="8" t="n">
-        <v>44.62500000000001</v>
-      </c>
-      <c r="AG273" s="8" t="n">
-        <v>12.75</v>
-      </c>
-      <c r="AH273" s="8" t="n">
-        <v>1332.375</v>
-      </c>
-      <c r="AI273" s="2" t="n"/>
-      <c r="AJ273" s="2" t="n"/>
-      <c r="AK273" s="8" t="n"/>
-      <c r="AL273" s="8" t="n"/>
-      <c r="AM273" s="8" t="n"/>
-      <c r="AN273" s="2" t="n"/>
-      <c r="AO273" s="2" t="n"/>
-      <c r="AP273" s="8" t="n"/>
-      <c r="AQ273" s="8" t="n"/>
-      <c r="AR273" s="8" t="n"/>
-      <c r="AS273" s="2" t="n"/>
-      <c r="AT273" s="2" t="n"/>
-      <c r="AU273" s="8" t="n"/>
-      <c r="AV273" s="8" t="n"/>
-      <c r="AW273" s="8" t="n"/>
-      <c r="AX273" s="2" t="n"/>
-      <c r="AY273" s="2" t="n"/>
-      <c r="AZ273" s="8" t="n"/>
-      <c r="BA273" s="8" t="n"/>
-      <c r="BB273" s="8" t="n"/>
-      <c r="BC273" s="2" t="n"/>
-      <c r="BD273" s="2" t="n"/>
-      <c r="BE273" s="8" t="n"/>
-      <c r="BF273" s="8" t="n"/>
-      <c r="BG273" s="8" t="n"/>
-      <c r="BH273" s="2" t="n"/>
-      <c r="BI273" s="2" t="n"/>
-      <c r="BJ273" s="8" t="n"/>
-      <c r="BK273" s="8" t="n"/>
-      <c r="BL273" s="8" t="n"/>
-      <c r="BM273" s="2" t="n"/>
-      <c r="BN273" s="2" t="n"/>
-    </row>
-    <row r="274">
-      <c r="A274" s="2" t="n"/>
-      <c r="B274" s="5" t="n"/>
-      <c r="C274" s="5" t="n"/>
-      <c r="D274" s="6" t="n"/>
-      <c r="E274" s="2" t="n"/>
-      <c r="F274" s="7" t="n"/>
-      <c r="G274" s="8" t="n"/>
-      <c r="H274" s="8" t="n"/>
-      <c r="I274" s="8" t="n"/>
-      <c r="J274" s="2" t="n"/>
-      <c r="K274" s="2" t="n"/>
-      <c r="L274" s="8" t="n"/>
-      <c r="M274" s="8" t="n"/>
-      <c r="N274" s="8" t="n"/>
-      <c r="O274" s="2" t="n"/>
-      <c r="P274" s="2" t="n"/>
-      <c r="Q274" s="8" t="n"/>
-      <c r="R274" s="8" t="n"/>
-      <c r="S274" s="8" t="n"/>
-      <c r="T274" s="2" t="n"/>
-      <c r="U274" s="2" t="n"/>
-      <c r="V274" s="8" t="n"/>
-      <c r="W274" s="8" t="n"/>
-      <c r="X274" s="8" t="n"/>
-      <c r="Y274" s="2" t="n"/>
-      <c r="Z274" s="2" t="n"/>
-      <c r="AA274" s="8" t="n">
-        <v>340</v>
-      </c>
-      <c r="AB274" s="8" t="n">
-        <v>11.9</v>
-      </c>
-      <c r="AC274" s="8" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="AD274" s="2" t="n">
-        <v>355.3</v>
-      </c>
-      <c r="AE274" s="2" t="n">
-        <v>1090</v>
-      </c>
-      <c r="AF274" s="8" t="n">
-        <v>38.15000000000001</v>
-      </c>
-      <c r="AG274" s="8" t="n">
-        <v>10.9</v>
-      </c>
-      <c r="AH274" s="8" t="n">
-        <v>1139.05</v>
-      </c>
-      <c r="AI274" s="2" t="n"/>
-      <c r="AJ274" s="2" t="n"/>
-      <c r="AK274" s="8" t="n"/>
-      <c r="AL274" s="8" t="n"/>
-      <c r="AM274" s="8" t="n"/>
-      <c r="AN274" s="2" t="n"/>
-      <c r="AO274" s="2" t="n"/>
-      <c r="AP274" s="8" t="n"/>
-      <c r="AQ274" s="8" t="n"/>
-      <c r="AR274" s="8" t="n"/>
-      <c r="AS274" s="2" t="n"/>
-      <c r="AT274" s="2" t="n"/>
-      <c r="AU274" s="8" t="n"/>
-      <c r="AV274" s="8" t="n"/>
-      <c r="AW274" s="8" t="n"/>
-      <c r="AX274" s="2" t="n"/>
-      <c r="AY274" s="2" t="n"/>
-      <c r="AZ274" s="8" t="n"/>
-      <c r="BA274" s="8" t="n"/>
-      <c r="BB274" s="8" t="n"/>
-      <c r="BC274" s="2" t="n"/>
-      <c r="BD274" s="2" t="n"/>
-      <c r="BE274" s="8" t="n"/>
-      <c r="BF274" s="8" t="n"/>
-      <c r="BG274" s="8" t="n"/>
-      <c r="BH274" s="2" t="n"/>
-      <c r="BI274" s="2" t="n"/>
-      <c r="BJ274" s="8" t="n"/>
-      <c r="BK274" s="8" t="n"/>
-      <c r="BL274" s="8" t="n"/>
-      <c r="BM274" s="2" t="n"/>
-      <c r="BN274" s="2" t="n"/>
-    </row>
-    <row r="275">
-      <c r="A275" s="2" t="n"/>
-      <c r="B275" s="5" t="n"/>
-      <c r="C275" s="5" t="n"/>
-      <c r="D275" s="6" t="n"/>
-      <c r="E275" s="2" t="n"/>
-      <c r="F275" s="7" t="n"/>
-      <c r="G275" s="8" t="n"/>
-      <c r="H275" s="8" t="n"/>
-      <c r="I275" s="8" t="n"/>
-      <c r="J275" s="2" t="n"/>
-      <c r="K275" s="2" t="n"/>
-      <c r="L275" s="8" t="n"/>
-      <c r="M275" s="8" t="n"/>
-      <c r="N275" s="8" t="n"/>
-      <c r="O275" s="2" t="n"/>
-      <c r="P275" s="2" t="n"/>
-      <c r="Q275" s="8" t="n"/>
-      <c r="R275" s="8" t="n"/>
-      <c r="S275" s="8" t="n"/>
-      <c r="T275" s="2" t="n"/>
-      <c r="U275" s="2" t="n"/>
-      <c r="V275" s="8" t="n"/>
-      <c r="W275" s="8" t="n"/>
-      <c r="X275" s="8" t="n"/>
-      <c r="Y275" s="2" t="n"/>
-      <c r="Z275" s="2" t="n"/>
-      <c r="AA275" s="8" t="n">
-        <v>4500</v>
-      </c>
-      <c r="AB275" s="8" t="n">
-        <v>157.5</v>
-      </c>
-      <c r="AC275" s="8" t="n">
-        <v>45</v>
-      </c>
-      <c r="AD275" s="2" t="n">
-        <v>4702.5</v>
-      </c>
-      <c r="AE275" s="2" t="n">
-        <v>2515</v>
-      </c>
-      <c r="AF275" s="8" t="n">
-        <v>88.02500000000001</v>
-      </c>
-      <c r="AG275" s="8" t="n">
-        <v>25.15</v>
-      </c>
-      <c r="AH275" s="8" t="n">
-        <v>2628.175</v>
-      </c>
-      <c r="AI275" s="2" t="n"/>
-      <c r="AJ275" s="2" t="n"/>
-      <c r="AK275" s="8" t="n"/>
-      <c r="AL275" s="8" t="n"/>
-      <c r="AM275" s="8" t="n"/>
-      <c r="AN275" s="2" t="n"/>
-      <c r="AO275" s="2" t="n"/>
-      <c r="AP275" s="8" t="n"/>
-      <c r="AQ275" s="8" t="n"/>
-      <c r="AR275" s="8" t="n"/>
-      <c r="AS275" s="2" t="n"/>
-      <c r="AT275" s="2" t="n"/>
-      <c r="AU275" s="8" t="n"/>
-      <c r="AV275" s="8" t="n"/>
-      <c r="AW275" s="8" t="n"/>
-      <c r="AX275" s="2" t="n"/>
-      <c r="AY275" s="2" t="n"/>
-      <c r="AZ275" s="8" t="n"/>
-      <c r="BA275" s="8" t="n"/>
-      <c r="BB275" s="8" t="n"/>
-      <c r="BC275" s="2" t="n"/>
-      <c r="BD275" s="2" t="n"/>
-      <c r="BE275" s="8" t="n"/>
-      <c r="BF275" s="8" t="n"/>
-      <c r="BG275" s="8" t="n"/>
-      <c r="BH275" s="2" t="n"/>
-      <c r="BI275" s="2" t="n"/>
-      <c r="BJ275" s="8" t="n"/>
-      <c r="BK275" s="8" t="n"/>
-      <c r="BL275" s="8" t="n"/>
-      <c r="BM275" s="2" t="n"/>
-      <c r="BN275" s="2" t="n"/>
-    </row>
-    <row r="276">
-      <c r="A276" s="2" t="n"/>
-      <c r="B276" s="5" t="n"/>
-      <c r="C276" s="5" t="n"/>
-      <c r="D276" s="6" t="n"/>
-      <c r="E276" s="2" t="n"/>
-      <c r="F276" s="7" t="n"/>
-      <c r="G276" s="8" t="n"/>
-      <c r="H276" s="8" t="n"/>
-      <c r="I276" s="8" t="n"/>
-      <c r="J276" s="2" t="n"/>
-      <c r="K276" s="2" t="n"/>
-      <c r="L276" s="8" t="n"/>
-      <c r="M276" s="8" t="n"/>
-      <c r="N276" s="8" t="n"/>
-      <c r="O276" s="2" t="n"/>
-      <c r="P276" s="2" t="n"/>
-      <c r="Q276" s="8" t="n"/>
-      <c r="R276" s="8" t="n"/>
-      <c r="S276" s="8" t="n"/>
-      <c r="T276" s="2" t="n"/>
-      <c r="U276" s="2" t="n"/>
-      <c r="V276" s="8" t="n"/>
-      <c r="W276" s="8" t="n"/>
-      <c r="X276" s="8" t="n"/>
-      <c r="Y276" s="2" t="n"/>
-      <c r="Z276" s="2" t="n"/>
-      <c r="AA276" s="8" t="n">
-        <v>510</v>
-      </c>
-      <c r="AB276" s="8" t="n">
-        <v>17.85</v>
-      </c>
-      <c r="AC276" s="8" t="n">
-        <v>5.100000000000001</v>
-      </c>
-      <c r="AD276" s="2" t="n">
-        <v>532.95</v>
-      </c>
-      <c r="AE276" s="2" t="n">
-        <v>1750</v>
-      </c>
-      <c r="AF276" s="8" t="n">
-        <v>61.25000000000001</v>
-      </c>
-      <c r="AG276" s="8" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="AH276" s="8" t="n">
-        <v>1828.75</v>
-      </c>
-      <c r="AI276" s="2" t="n"/>
-      <c r="AJ276" s="2" t="n"/>
-      <c r="AK276" s="8" t="n"/>
-      <c r="AL276" s="8" t="n"/>
-      <c r="AM276" s="8" t="n"/>
-      <c r="AN276" s="2" t="n"/>
-      <c r="AO276" s="2" t="n"/>
-      <c r="AP276" s="8" t="n"/>
-      <c r="AQ276" s="8" t="n"/>
-      <c r="AR276" s="8" t="n"/>
-      <c r="AS276" s="2" t="n"/>
-      <c r="AT276" s="2" t="n"/>
-      <c r="AU276" s="8" t="n"/>
-      <c r="AV276" s="8" t="n"/>
-      <c r="AW276" s="8" t="n"/>
-      <c r="AX276" s="2" t="n"/>
-      <c r="AY276" s="2" t="n"/>
-      <c r="AZ276" s="8" t="n"/>
-      <c r="BA276" s="8" t="n"/>
-      <c r="BB276" s="8" t="n"/>
-      <c r="BC276" s="2" t="n"/>
-      <c r="BD276" s="2" t="n"/>
-      <c r="BE276" s="8" t="n"/>
-      <c r="BF276" s="8" t="n"/>
-      <c r="BG276" s="8" t="n"/>
-      <c r="BH276" s="2" t="n"/>
-      <c r="BI276" s="2" t="n"/>
-      <c r="BJ276" s="8" t="n"/>
-      <c r="BK276" s="8" t="n"/>
-      <c r="BL276" s="8" t="n"/>
-      <c r="BM276" s="2" t="n"/>
-      <c r="BN276" s="2" t="n"/>
-    </row>
-    <row r="277">
-      <c r="A277" s="2" t="n"/>
-      <c r="B277" s="5" t="n"/>
-      <c r="C277" s="5" t="n"/>
-      <c r="D277" s="6" t="n"/>
-      <c r="E277" s="2" t="n"/>
-      <c r="F277" s="7" t="n"/>
-      <c r="G277" s="8" t="n"/>
-      <c r="H277" s="8" t="n"/>
-      <c r="I277" s="8" t="n"/>
-      <c r="J277" s="2" t="n"/>
-      <c r="K277" s="2" t="n"/>
-      <c r="L277" s="8" t="n"/>
-      <c r="M277" s="8" t="n"/>
-      <c r="N277" s="8" t="n"/>
-      <c r="O277" s="2" t="n"/>
-      <c r="P277" s="2" t="n"/>
-      <c r="Q277" s="8" t="n"/>
-      <c r="R277" s="8" t="n"/>
-      <c r="S277" s="8" t="n"/>
-      <c r="T277" s="2" t="n"/>
-      <c r="U277" s="2" t="n"/>
-      <c r="V277" s="8" t="n"/>
-      <c r="W277" s="8" t="n"/>
-      <c r="X277" s="8" t="n"/>
-      <c r="Y277" s="2" t="n"/>
-      <c r="Z277" s="2" t="n"/>
-      <c r="AA277" s="8" t="n">
-        <v>640</v>
-      </c>
-      <c r="AB277" s="8" t="n">
-        <v>22.4</v>
-      </c>
-      <c r="AC277" s="8" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="AD277" s="2" t="n">
-        <v>668.8</v>
-      </c>
-      <c r="AE277" s="2" t="n">
-        <v>1980</v>
-      </c>
-      <c r="AF277" s="8" t="n">
-        <v>69.30000000000001</v>
-      </c>
-      <c r="AG277" s="8" t="n">
-        <v>19.8</v>
-      </c>
-      <c r="AH277" s="8" t="n">
-        <v>2069.1</v>
-      </c>
-      <c r="AI277" s="2" t="n"/>
-      <c r="AJ277" s="2" t="n"/>
-      <c r="AK277" s="8" t="n"/>
-      <c r="AL277" s="8" t="n"/>
-      <c r="AM277" s="8" t="n"/>
-      <c r="AN277" s="2" t="n"/>
-      <c r="AO277" s="2" t="n"/>
-      <c r="AP277" s="8" t="n"/>
-      <c r="AQ277" s="8" t="n"/>
-      <c r="AR277" s="8" t="n"/>
-      <c r="AS277" s="2" t="n"/>
-      <c r="AT277" s="2" t="n"/>
-      <c r="AU277" s="8" t="n"/>
-      <c r="AV277" s="8" t="n"/>
-      <c r="AW277" s="8" t="n"/>
-      <c r="AX277" s="2" t="n"/>
-      <c r="AY277" s="2" t="n"/>
-      <c r="AZ277" s="8" t="n"/>
-      <c r="BA277" s="8" t="n"/>
-      <c r="BB277" s="8" t="n"/>
-      <c r="BC277" s="2" t="n"/>
-      <c r="BD277" s="2" t="n"/>
-      <c r="BE277" s="8" t="n"/>
-      <c r="BF277" s="8" t="n"/>
-      <c r="BG277" s="8" t="n"/>
-      <c r="BH277" s="2" t="n"/>
-      <c r="BI277" s="2" t="n"/>
-      <c r="BJ277" s="8" t="n"/>
-      <c r="BK277" s="8" t="n"/>
-      <c r="BL277" s="8" t="n"/>
-      <c r="BM277" s="2" t="n"/>
-      <c r="BN277" s="2" t="n"/>
-    </row>
-    <row r="278">
-      <c r="A278" s="2" t="n"/>
-      <c r="B278" s="5" t="n"/>
-      <c r="C278" s="5" t="n"/>
-      <c r="D278" s="6" t="n"/>
-      <c r="E278" s="2" t="n"/>
-      <c r="F278" s="7" t="n"/>
-      <c r="G278" s="8" t="n"/>
-      <c r="H278" s="8" t="n"/>
-      <c r="I278" s="8" t="n"/>
-      <c r="J278" s="2" t="n"/>
-      <c r="K278" s="2" t="n"/>
-      <c r="L278" s="8" t="n"/>
-      <c r="M278" s="8" t="n"/>
-      <c r="N278" s="8" t="n"/>
-      <c r="O278" s="2" t="n"/>
-      <c r="P278" s="2" t="n"/>
-      <c r="Q278" s="8" t="n"/>
-      <c r="R278" s="8" t="n"/>
-      <c r="S278" s="8" t="n"/>
-      <c r="T278" s="2" t="n"/>
-      <c r="U278" s="2" t="n"/>
-      <c r="V278" s="8" t="n"/>
-      <c r="W278" s="8" t="n"/>
-      <c r="X278" s="8" t="n"/>
-      <c r="Y278" s="2" t="n"/>
-      <c r="Z278" s="2" t="n"/>
-      <c r="AA278" s="8" t="n">
-        <v>650</v>
-      </c>
-      <c r="AB278" s="8" t="n">
-        <v>22.75</v>
-      </c>
-      <c r="AC278" s="8" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="AD278" s="2" t="n">
-        <v>679.25</v>
-      </c>
-      <c r="AE278" s="2" t="n">
-        <v>1980</v>
-      </c>
-      <c r="AF278" s="8" t="n">
-        <v>69.30000000000001</v>
-      </c>
-      <c r="AG278" s="8" t="n">
-        <v>19.8</v>
-      </c>
-      <c r="AH278" s="8" t="n">
-        <v>2069.1</v>
-      </c>
-      <c r="AI278" s="2" t="n"/>
-      <c r="AJ278" s="2" t="n"/>
-      <c r="AK278" s="8" t="n"/>
-      <c r="AL278" s="8" t="n"/>
-      <c r="AM278" s="8" t="n"/>
-      <c r="AN278" s="2" t="n"/>
-      <c r="AO278" s="2" t="n"/>
-      <c r="AP278" s="8" t="n"/>
-      <c r="AQ278" s="8" t="n"/>
-      <c r="AR278" s="8" t="n"/>
-      <c r="AS278" s="2" t="n"/>
-      <c r="AT278" s="2" t="n"/>
-      <c r="AU278" s="8" t="n"/>
-      <c r="AV278" s="8" t="n"/>
-      <c r="AW278" s="8" t="n"/>
-      <c r="AX278" s="2" t="n"/>
-      <c r="AY278" s="2" t="n"/>
-      <c r="AZ278" s="8" t="n"/>
-      <c r="BA278" s="8" t="n"/>
-      <c r="BB278" s="8" t="n"/>
-      <c r="BC278" s="2" t="n"/>
-      <c r="BD278" s="2" t="n"/>
-      <c r="BE278" s="8" t="n"/>
-      <c r="BF278" s="8" t="n"/>
-      <c r="BG278" s="8" t="n"/>
-      <c r="BH278" s="2" t="n"/>
-      <c r="BI278" s="2" t="n"/>
-      <c r="BJ278" s="8" t="n"/>
-      <c r="BK278" s="8" t="n"/>
-      <c r="BL278" s="8" t="n"/>
-      <c r="BM278" s="2" t="n"/>
-      <c r="BN278" s="2" t="n"/>
-    </row>
-    <row r="279">
-      <c r="A279" s="2" t="n"/>
-      <c r="B279" s="5" t="n"/>
-      <c r="C279" s="5" t="n"/>
-      <c r="D279" s="6" t="n"/>
-      <c r="E279" s="2" t="n"/>
-      <c r="F279" s="7" t="n"/>
-      <c r="G279" s="8" t="n"/>
-      <c r="H279" s="8" t="n"/>
-      <c r="I279" s="8" t="n"/>
-      <c r="J279" s="2" t="n"/>
-      <c r="K279" s="2" t="n"/>
-      <c r="L279" s="8" t="n"/>
-      <c r="M279" s="8" t="n"/>
-      <c r="N279" s="8" t="n"/>
-      <c r="O279" s="2" t="n"/>
-      <c r="P279" s="2" t="n"/>
-      <c r="Q279" s="8" t="n"/>
-      <c r="R279" s="8" t="n"/>
-      <c r="S279" s="8" t="n"/>
-      <c r="T279" s="2" t="n"/>
-      <c r="U279" s="2" t="n"/>
-      <c r="V279" s="8" t="n"/>
-      <c r="W279" s="8" t="n"/>
-      <c r="X279" s="8" t="n"/>
-      <c r="Y279" s="2" t="n"/>
-      <c r="Z279" s="2" t="n"/>
-      <c r="AA279" s="8" t="n">
-        <v>2200</v>
-      </c>
-      <c r="AB279" s="8" t="n">
-        <v>77.00000000000001</v>
-      </c>
-      <c r="AC279" s="8" t="n">
-        <v>22</v>
-      </c>
-      <c r="AD279" s="2" t="n">
-        <v>2299</v>
-      </c>
-      <c r="AE279" s="2" t="n">
-        <v>1250</v>
-      </c>
-      <c r="AF279" s="8" t="n">
-        <v>43.75000000000001</v>
-      </c>
-      <c r="AG279" s="8" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="AH279" s="8" t="n">
-        <v>1306.25</v>
-      </c>
-      <c r="AI279" s="2" t="n"/>
-      <c r="AJ279" s="2" t="n"/>
-      <c r="AK279" s="8" t="n"/>
-      <c r="AL279" s="8" t="n"/>
-      <c r="AM279" s="8" t="n"/>
-      <c r="AN279" s="2" t="n"/>
-      <c r="AO279" s="2" t="n"/>
-      <c r="AP279" s="8" t="n"/>
-      <c r="AQ279" s="8" t="n"/>
-      <c r="AR279" s="8" t="n"/>
-      <c r="AS279" s="2" t="n"/>
-      <c r="AT279" s="2" t="n"/>
-      <c r="AU279" s="8" t="n"/>
-      <c r="AV279" s="8" t="n"/>
-      <c r="AW279" s="8" t="n"/>
-      <c r="AX279" s="2" t="n"/>
-      <c r="AY279" s="2" t="n"/>
-      <c r="AZ279" s="8" t="n"/>
-      <c r="BA279" s="8" t="n"/>
-      <c r="BB279" s="8" t="n"/>
-      <c r="BC279" s="2" t="n"/>
-      <c r="BD279" s="2" t="n"/>
-      <c r="BE279" s="8" t="n"/>
-      <c r="BF279" s="8" t="n"/>
-      <c r="BG279" s="8" t="n"/>
-      <c r="BH279" s="2" t="n"/>
-      <c r="BI279" s="2" t="n"/>
-      <c r="BJ279" s="8" t="n"/>
-      <c r="BK279" s="8" t="n"/>
-      <c r="BL279" s="8" t="n"/>
-      <c r="BM279" s="2" t="n"/>
-      <c r="BN279" s="2" t="n"/>
-    </row>
-    <row r="280">
-      <c r="A280" s="2" t="n"/>
-      <c r="B280" s="5" t="n"/>
-      <c r="C280" s="5" t="n"/>
-      <c r="D280" s="6" t="n"/>
-      <c r="E280" s="2" t="n"/>
-      <c r="F280" s="7" t="n"/>
-      <c r="G280" s="8" t="n"/>
-      <c r="H280" s="8" t="n"/>
-      <c r="I280" s="8" t="n"/>
-      <c r="J280" s="2" t="n"/>
-      <c r="K280" s="2" t="n"/>
-      <c r="L280" s="8" t="n"/>
-      <c r="M280" s="8" t="n"/>
-      <c r="N280" s="8" t="n"/>
-      <c r="O280" s="2" t="n"/>
-      <c r="P280" s="2" t="n"/>
-      <c r="Q280" s="8" t="n"/>
-      <c r="R280" s="8" t="n"/>
-      <c r="S280" s="8" t="n"/>
-      <c r="T280" s="2" t="n"/>
-      <c r="U280" s="2" t="n"/>
-      <c r="V280" s="8" t="n"/>
-      <c r="W280" s="8" t="n"/>
-      <c r="X280" s="8" t="n"/>
-      <c r="Y280" s="2" t="n"/>
-      <c r="Z280" s="2" t="n"/>
-      <c r="AA280" s="8" t="n"/>
-      <c r="AB280" s="8" t="n"/>
-      <c r="AC280" s="8" t="n"/>
-      <c r="AD280" s="2" t="n"/>
-      <c r="AE280" s="2" t="n">
-        <v>1505</v>
-      </c>
-      <c r="AF280" s="8" t="n">
-        <v>52.675</v>
-      </c>
-      <c r="AG280" s="8" t="n">
-        <v>15.05</v>
-      </c>
-      <c r="AH280" s="8" t="n">
-        <v>1572.725</v>
-      </c>
-      <c r="AI280" s="2" t="n"/>
-      <c r="AJ280" s="2" t="n"/>
-      <c r="AK280" s="8" t="n"/>
-      <c r="AL280" s="8" t="n"/>
-      <c r="AM280" s="8" t="n"/>
-      <c r="AN280" s="2" t="n"/>
-      <c r="AO280" s="2" t="n"/>
-      <c r="AP280" s="8" t="n"/>
-      <c r="AQ280" s="8" t="n"/>
-      <c r="AR280" s="8" t="n"/>
-      <c r="AS280" s="2" t="n"/>
-      <c r="AT280" s="2" t="n"/>
-      <c r="AU280" s="8" t="n"/>
-      <c r="AV280" s="8" t="n"/>
-      <c r="AW280" s="8" t="n"/>
-      <c r="AX280" s="2" t="n"/>
-      <c r="AY280" s="2" t="n"/>
-      <c r="AZ280" s="8" t="n"/>
-      <c r="BA280" s="8" t="n"/>
-      <c r="BB280" s="8" t="n"/>
-      <c r="BC280" s="2" t="n"/>
-      <c r="BD280" s="2" t="n"/>
-      <c r="BE280" s="8" t="n"/>
-      <c r="BF280" s="8" t="n"/>
-      <c r="BG280" s="8" t="n"/>
-      <c r="BH280" s="2" t="n"/>
-      <c r="BI280" s="2" t="n"/>
-      <c r="BJ280" s="8" t="n"/>
-      <c r="BK280" s="8" t="n"/>
-      <c r="BL280" s="8" t="n"/>
-      <c r="BM280" s="2" t="n"/>
-      <c r="BN280" s="2" t="n"/>
-    </row>
-    <row r="281">
-      <c r="A281" s="2" t="n"/>
-      <c r="B281" s="5" t="n"/>
-      <c r="C281" s="5" t="n"/>
-      <c r="D281" s="6" t="n"/>
-      <c r="E281" s="2" t="n"/>
-      <c r="F281" s="7" t="n"/>
-      <c r="G281" s="8" t="n"/>
-      <c r="H281" s="8" t="n"/>
-      <c r="I281" s="8" t="n"/>
-      <c r="J281" s="2" t="n"/>
-      <c r="K281" s="2" t="n"/>
-      <c r="L281" s="8" t="n"/>
-      <c r="M281" s="8" t="n"/>
-      <c r="N281" s="8" t="n"/>
-      <c r="O281" s="2" t="n"/>
-      <c r="P281" s="2" t="n"/>
-      <c r="Q281" s="8" t="n"/>
-      <c r="R281" s="8" t="n"/>
-      <c r="S281" s="8" t="n"/>
-      <c r="T281" s="2" t="n"/>
-      <c r="U281" s="2" t="n"/>
-      <c r="V281" s="8" t="n"/>
-      <c r="W281" s="8" t="n"/>
-      <c r="X281" s="8" t="n"/>
-      <c r="Y281" s="2" t="n"/>
-      <c r="Z281" s="2" t="n"/>
-      <c r="AA281" s="8" t="n"/>
-      <c r="AB281" s="8" t="n"/>
-      <c r="AC281" s="8" t="n"/>
-      <c r="AD281" s="2" t="n"/>
-      <c r="AE281" s="2" t="n">
-        <v>1230</v>
-      </c>
-      <c r="AF281" s="8" t="n">
-        <v>43.05</v>
-      </c>
-      <c r="AG281" s="8" t="n">
-        <v>12.3</v>
-      </c>
-      <c r="AH281" s="8" t="n">
-        <v>1285.35</v>
-      </c>
-      <c r="AI281" s="2" t="n"/>
-      <c r="AJ281" s="2" t="n"/>
-      <c r="AK281" s="8" t="n"/>
-      <c r="AL281" s="8" t="n"/>
-      <c r="AM281" s="8" t="n"/>
-      <c r="AN281" s="2" t="n"/>
-      <c r="AO281" s="2" t="n"/>
-      <c r="AP281" s="8" t="n"/>
-      <c r="AQ281" s="8" t="n"/>
-      <c r="AR281" s="8" t="n"/>
-      <c r="AS281" s="2" t="n"/>
-      <c r="AT281" s="2" t="n"/>
-      <c r="AU281" s="8" t="n"/>
-      <c r="AV281" s="8" t="n"/>
-      <c r="AW281" s="8" t="n"/>
-      <c r="AX281" s="2" t="n"/>
-      <c r="AY281" s="2" t="n"/>
-      <c r="AZ281" s="8" t="n"/>
-      <c r="BA281" s="8" t="n"/>
-      <c r="BB281" s="8" t="n"/>
-      <c r="BC281" s="2" t="n"/>
-      <c r="BD281" s="2" t="n"/>
-      <c r="BE281" s="8" t="n"/>
-      <c r="BF281" s="8" t="n"/>
-      <c r="BG281" s="8" t="n"/>
-      <c r="BH281" s="2" t="n"/>
-      <c r="BI281" s="2" t="n"/>
-      <c r="BJ281" s="8" t="n"/>
-      <c r="BK281" s="8" t="n"/>
-      <c r="BL281" s="8" t="n"/>
-      <c r="BM281" s="2" t="n"/>
-      <c r="BN281" s="2" t="n"/>
-    </row>
-    <row r="282">
-      <c r="A282" s="2" t="n"/>
-      <c r="B282" s="5" t="n"/>
-      <c r="C282" s="5" t="n"/>
-      <c r="D282" s="6" t="n"/>
-      <c r="E282" s="2" t="n"/>
-      <c r="F282" s="7" t="n"/>
-      <c r="G282" s="8" t="n"/>
-      <c r="H282" s="8" t="n"/>
-      <c r="I282" s="8" t="n"/>
-      <c r="J282" s="2" t="n"/>
-      <c r="K282" s="2" t="n"/>
-      <c r="L282" s="8" t="n"/>
-      <c r="M282" s="8" t="n"/>
-      <c r="N282" s="8" t="n"/>
-      <c r="O282" s="2" t="n"/>
-      <c r="P282" s="2" t="n"/>
-      <c r="Q282" s="8" t="n"/>
-      <c r="R282" s="8" t="n"/>
-      <c r="S282" s="8" t="n"/>
-      <c r="T282" s="2" t="n"/>
-      <c r="U282" s="2" t="n"/>
-      <c r="V282" s="8" t="n"/>
-      <c r="W282" s="8" t="n"/>
-      <c r="X282" s="8" t="n"/>
-      <c r="Y282" s="2" t="n"/>
-      <c r="Z282" s="2" t="n"/>
-      <c r="AA282" s="8" t="n"/>
-      <c r="AB282" s="8" t="n"/>
-      <c r="AC282" s="8" t="n"/>
-      <c r="AD282" s="2" t="n"/>
-      <c r="AE282" s="2" t="n">
-        <v>3755</v>
-      </c>
-      <c r="AF282" s="8" t="n">
-        <v>131.425</v>
-      </c>
-      <c r="AG282" s="8" t="n">
-        <v>37.55</v>
-      </c>
-      <c r="AH282" s="8" t="n">
-        <v>3923.975</v>
-      </c>
-      <c r="AI282" s="2" t="n"/>
-      <c r="AJ282" s="2" t="n"/>
-      <c r="AK282" s="8" t="n"/>
-      <c r="AL282" s="8" t="n"/>
-      <c r="AM282" s="8" t="n"/>
-      <c r="AN282" s="2" t="n"/>
-      <c r="AO282" s="2" t="n"/>
-      <c r="AP282" s="8" t="n"/>
-      <c r="AQ282" s="8" t="n"/>
-      <c r="AR282" s="8" t="n"/>
-      <c r="AS282" s="2" t="n"/>
-      <c r="AT282" s="2" t="n"/>
-      <c r="AU282" s="8" t="n"/>
-      <c r="AV282" s="8" t="n"/>
-      <c r="AW282" s="8" t="n"/>
-      <c r="AX282" s="2" t="n"/>
-      <c r="AY282" s="2" t="n"/>
-      <c r="AZ282" s="8" t="n"/>
-      <c r="BA282" s="8" t="n"/>
-      <c r="BB282" s="8" t="n"/>
-      <c r="BC282" s="2" t="n"/>
-      <c r="BD282" s="2" t="n"/>
-      <c r="BE282" s="8" t="n"/>
-      <c r="BF282" s="8" t="n"/>
-      <c r="BG282" s="8" t="n"/>
-      <c r="BH282" s="2" t="n"/>
-      <c r="BI282" s="2" t="n"/>
-      <c r="BJ282" s="8" t="n"/>
-      <c r="BK282" s="8" t="n"/>
-      <c r="BL282" s="8" t="n"/>
-      <c r="BM282" s="2" t="n"/>
-      <c r="BN282" s="2" t="n"/>
-    </row>
-    <row r="283">
-      <c r="A283" s="2" t="n"/>
-      <c r="B283" s="5" t="n"/>
-      <c r="C283" s="5" t="n"/>
-      <c r="D283" s="6" t="n"/>
-      <c r="E283" s="2" t="n"/>
-      <c r="F283" s="7" t="n"/>
-      <c r="G283" s="8" t="n"/>
-      <c r="H283" s="8" t="n"/>
-      <c r="I283" s="8" t="n"/>
-      <c r="J283" s="2" t="n"/>
-      <c r="K283" s="2" t="n"/>
-      <c r="L283" s="8" t="n"/>
-      <c r="M283" s="8" t="n"/>
-      <c r="N283" s="8" t="n"/>
-      <c r="O283" s="2" t="n"/>
-      <c r="P283" s="2" t="n"/>
-      <c r="Q283" s="8" t="n"/>
-      <c r="R283" s="8" t="n"/>
-      <c r="S283" s="8" t="n"/>
-      <c r="T283" s="2" t="n"/>
-      <c r="U283" s="2" t="n"/>
-      <c r="V283" s="8" t="n"/>
-      <c r="W283" s="8" t="n"/>
-      <c r="X283" s="8" t="n"/>
-      <c r="Y283" s="2" t="n"/>
-      <c r="Z283" s="2" t="n"/>
-      <c r="AA283" s="8" t="n"/>
-      <c r="AB283" s="8" t="n"/>
-      <c r="AC283" s="8" t="n"/>
-      <c r="AD283" s="2" t="n"/>
-      <c r="AE283" s="2" t="n">
-        <v>8850</v>
-      </c>
-      <c r="AF283" s="8" t="n">
-        <v>309.7500000000001</v>
-      </c>
-      <c r="AG283" s="8" t="n">
-        <v>88.5</v>
-      </c>
-      <c r="AH283" s="8" t="n">
-        <v>9248.25</v>
-      </c>
-      <c r="AI283" s="2" t="n"/>
-      <c r="AJ283" s="2" t="n"/>
-      <c r="AK283" s="8" t="n"/>
-      <c r="AL283" s="8" t="n"/>
-      <c r="AM283" s="8" t="n"/>
-      <c r="AN283" s="2" t="n"/>
-      <c r="AO283" s="2" t="n"/>
-      <c r="AP283" s="8" t="n"/>
-      <c r="AQ283" s="8" t="n"/>
-      <c r="AR283" s="8" t="n"/>
-      <c r="AS283" s="2" t="n"/>
-      <c r="AT283" s="2" t="n"/>
-      <c r="AU283" s="8" t="n"/>
-      <c r="AV283" s="8" t="n"/>
-      <c r="AW283" s="8" t="n"/>
-      <c r="AX283" s="2" t="n"/>
-      <c r="AY283" s="2" t="n"/>
-      <c r="AZ283" s="8" t="n"/>
-      <c r="BA283" s="8" t="n"/>
-      <c r="BB283" s="8" t="n"/>
-      <c r="BC283" s="2" t="n"/>
-      <c r="BD283" s="2" t="n"/>
-      <c r="BE283" s="8" t="n"/>
-      <c r="BF283" s="8" t="n"/>
-      <c r="BG283" s="8" t="n"/>
-      <c r="BH283" s="2" t="n"/>
-      <c r="BI283" s="2" t="n"/>
-      <c r="BJ283" s="8" t="n"/>
-      <c r="BK283" s="8" t="n"/>
-      <c r="BL283" s="8" t="n"/>
-      <c r="BM283" s="2" t="n"/>
-      <c r="BN283" s="2" t="n"/>
-    </row>
-    <row r="284">
-      <c r="A284" s="2" t="n"/>
-      <c r="B284" s="5" t="n"/>
-      <c r="C284" s="5" t="n"/>
-      <c r="D284" s="6" t="n"/>
-      <c r="E284" s="2" t="n"/>
-      <c r="F284" s="7" t="n"/>
-      <c r="G284" s="8" t="n"/>
-      <c r="H284" s="8" t="n"/>
-      <c r="I284" s="8" t="n"/>
-      <c r="J284" s="2" t="n"/>
-      <c r="K284" s="2" t="n"/>
-      <c r="L284" s="8" t="n"/>
-      <c r="M284" s="8" t="n"/>
-      <c r="N284" s="8" t="n"/>
-      <c r="O284" s="2" t="n"/>
-      <c r="P284" s="2" t="n"/>
-      <c r="Q284" s="8" t="n"/>
-      <c r="R284" s="8" t="n"/>
-      <c r="S284" s="8" t="n"/>
-      <c r="T284" s="2" t="n"/>
-      <c r="U284" s="2" t="n"/>
-      <c r="V284" s="8" t="n"/>
-      <c r="W284" s="8" t="n"/>
-      <c r="X284" s="8" t="n"/>
-      <c r="Y284" s="2" t="n"/>
-      <c r="Z284" s="2" t="n"/>
-      <c r="AA284" s="8" t="n"/>
-      <c r="AB284" s="8" t="n"/>
-      <c r="AC284" s="8" t="n"/>
-      <c r="AD284" s="2" t="n"/>
-      <c r="AE284" s="2" t="n">
-        <v>1730</v>
-      </c>
-      <c r="AF284" s="8" t="n">
-        <v>60.55</v>
-      </c>
-      <c r="AG284" s="8" t="n">
-        <v>17.3</v>
-      </c>
-      <c r="AH284" s="8" t="n">
-        <v>1807.85</v>
-      </c>
-      <c r="AI284" s="2" t="n"/>
-      <c r="AJ284" s="2" t="n"/>
-      <c r="AK284" s="8" t="n"/>
-      <c r="AL284" s="8" t="n"/>
-      <c r="AM284" s="8" t="n"/>
-      <c r="AN284" s="2" t="n"/>
-      <c r="AO284" s="2" t="n"/>
-      <c r="AP284" s="8" t="n"/>
-      <c r="AQ284" s="8" t="n"/>
-      <c r="AR284" s="8" t="n"/>
-      <c r="AS284" s="2" t="n"/>
-      <c r="AT284" s="2" t="n"/>
-      <c r="AU284" s="8" t="n"/>
-      <c r="AV284" s="8" t="n"/>
-      <c r="AW284" s="8" t="n"/>
-      <c r="AX284" s="2" t="n"/>
-      <c r="AY284" s="2" t="n"/>
-      <c r="AZ284" s="8" t="n"/>
-      <c r="BA284" s="8" t="n"/>
-      <c r="BB284" s="8" t="n"/>
-      <c r="BC284" s="2" t="n"/>
-      <c r="BD284" s="2" t="n"/>
-      <c r="BE284" s="8" t="n"/>
-      <c r="BF284" s="8" t="n"/>
-      <c r="BG284" s="8" t="n"/>
-      <c r="BH284" s="2" t="n"/>
-      <c r="BI284" s="2" t="n"/>
-      <c r="BJ284" s="8" t="n"/>
-      <c r="BK284" s="8" t="n"/>
-      <c r="BL284" s="8" t="n"/>
-      <c r="BM284" s="2" t="n"/>
-      <c r="BN284" s="2" t="n"/>
-    </row>
-    <row r="285">
-      <c r="A285" s="2" t="n"/>
-      <c r="B285" s="5" t="n"/>
-      <c r="C285" s="5" t="n"/>
-      <c r="D285" s="6" t="n"/>
-      <c r="E285" s="2" t="n"/>
-      <c r="F285" s="7" t="n"/>
-      <c r="G285" s="8" t="n"/>
-      <c r="H285" s="8" t="n"/>
-      <c r="I285" s="8" t="n"/>
-      <c r="J285" s="2" t="n"/>
-      <c r="K285" s="2" t="n"/>
-      <c r="L285" s="8" t="n"/>
-      <c r="M285" s="8" t="n"/>
-      <c r="N285" s="8" t="n"/>
-      <c r="O285" s="2" t="n"/>
-      <c r="P285" s="2" t="n"/>
-      <c r="Q285" s="8" t="n"/>
-      <c r="R285" s="8" t="n"/>
-      <c r="S285" s="8" t="n"/>
-      <c r="T285" s="2" t="n"/>
-      <c r="U285" s="2" t="n"/>
-      <c r="V285" s="8" t="n"/>
-      <c r="W285" s="8" t="n"/>
-      <c r="X285" s="8" t="n"/>
-      <c r="Y285" s="2" t="n"/>
-      <c r="Z285" s="2" t="n"/>
-      <c r="AA285" s="8" t="n"/>
-      <c r="AB285" s="8" t="n"/>
-      <c r="AC285" s="8" t="n"/>
-      <c r="AD285" s="2" t="n"/>
-      <c r="AE285" s="2" t="n">
-        <v>5700</v>
-      </c>
-      <c r="AF285" s="8" t="n">
-        <v>199.5</v>
-      </c>
-      <c r="AG285" s="8" t="n">
-        <v>57</v>
-      </c>
-      <c r="AH285" s="8" t="n">
-        <v>5956.5</v>
-      </c>
-      <c r="AI285" s="2" t="n"/>
-      <c r="AJ285" s="2" t="n"/>
-      <c r="AK285" s="8" t="n"/>
-      <c r="AL285" s="8" t="n"/>
-      <c r="AM285" s="8" t="n"/>
-      <c r="AN285" s="2" t="n"/>
-      <c r="AO285" s="2" t="n"/>
-      <c r="AP285" s="8" t="n"/>
-      <c r="AQ285" s="8" t="n"/>
-      <c r="AR285" s="8" t="n"/>
-      <c r="AS285" s="2" t="n"/>
-      <c r="AT285" s="2" t="n"/>
-      <c r="AU285" s="8" t="n"/>
-      <c r="AV285" s="8" t="n"/>
-      <c r="AW285" s="8" t="n"/>
-      <c r="AX285" s="2" t="n"/>
-      <c r="AY285" s="2" t="n"/>
-      <c r="AZ285" s="8" t="n"/>
-      <c r="BA285" s="8" t="n"/>
-      <c r="BB285" s="8" t="n"/>
-      <c r="BC285" s="2" t="n"/>
-      <c r="BD285" s="2" t="n"/>
-      <c r="BE285" s="8" t="n"/>
-      <c r="BF285" s="8" t="n"/>
-      <c r="BG285" s="8" t="n"/>
-      <c r="BH285" s="2" t="n"/>
-      <c r="BI285" s="2" t="n"/>
-      <c r="BJ285" s="8" t="n"/>
-      <c r="BK285" s="8" t="n"/>
-      <c r="BL285" s="8" t="n"/>
-      <c r="BM285" s="2" t="n"/>
-      <c r="BN285" s="2" t="n"/>
-    </row>
-    <row r="286">
-      <c r="A286" s="2" t="n"/>
-      <c r="B286" s="5" t="n"/>
-      <c r="C286" s="5" t="n"/>
-      <c r="D286" s="6" t="n"/>
-      <c r="E286" s="2" t="n"/>
-      <c r="F286" s="7" t="n"/>
-      <c r="G286" s="8" t="n"/>
-      <c r="H286" s="8" t="n"/>
-      <c r="I286" s="8" t="n"/>
-      <c r="J286" s="2" t="n"/>
-      <c r="K286" s="2" t="n"/>
-      <c r="L286" s="8" t="n"/>
-      <c r="M286" s="8" t="n"/>
-      <c r="N286" s="8" t="n"/>
-      <c r="O286" s="2" t="n"/>
-      <c r="P286" s="2" t="n"/>
-      <c r="Q286" s="8" t="n"/>
-      <c r="R286" s="8" t="n"/>
-      <c r="S286" s="8" t="n"/>
-      <c r="T286" s="2" t="n"/>
-      <c r="U286" s="2" t="n"/>
-      <c r="V286" s="8" t="n"/>
-      <c r="W286" s="8" t="n"/>
-      <c r="X286" s="8" t="n"/>
-      <c r="Y286" s="2" t="n"/>
-      <c r="Z286" s="2" t="n"/>
-      <c r="AA286" s="8" t="n"/>
-      <c r="AB286" s="8" t="n"/>
-      <c r="AC286" s="8" t="n"/>
-      <c r="AD286" s="2" t="n"/>
-      <c r="AE286" s="2" t="n">
-        <v>3200</v>
-      </c>
-      <c r="AF286" s="8" t="n">
-        <v>112</v>
-      </c>
-      <c r="AG286" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="AH286" s="8" t="n">
-        <v>3344</v>
-      </c>
-      <c r="AI286" s="2" t="n"/>
-      <c r="AJ286" s="2" t="n"/>
-      <c r="AK286" s="8" t="n"/>
-      <c r="AL286" s="8" t="n"/>
-      <c r="AM286" s="8" t="n"/>
-      <c r="AN286" s="2" t="n"/>
-      <c r="AO286" s="2" t="n"/>
-      <c r="AP286" s="8" t="n"/>
-      <c r="AQ286" s="8" t="n"/>
-      <c r="AR286" s="8" t="n"/>
-      <c r="AS286" s="2" t="n"/>
-      <c r="AT286" s="2" t="n"/>
-      <c r="AU286" s="8" t="n"/>
-      <c r="AV286" s="8" t="n"/>
-      <c r="AW286" s="8" t="n"/>
-      <c r="AX286" s="2" t="n"/>
-      <c r="AY286" s="2" t="n"/>
-      <c r="AZ286" s="8" t="n"/>
-      <c r="BA286" s="8" t="n"/>
-      <c r="BB286" s="8" t="n"/>
-      <c r="BC286" s="2" t="n"/>
-      <c r="BD286" s="2" t="n"/>
-      <c r="BE286" s="8" t="n"/>
-      <c r="BF286" s="8" t="n"/>
-      <c r="BG286" s="8" t="n"/>
-      <c r="BH286" s="2" t="n"/>
-      <c r="BI286" s="2" t="n"/>
-      <c r="BJ286" s="8" t="n"/>
-      <c r="BK286" s="8" t="n"/>
-      <c r="BL286" s="8" t="n"/>
-      <c r="BM286" s="2" t="n"/>
-      <c r="BN286" s="2" t="n"/>
-    </row>
-    <row r="287">
-      <c r="A287" s="2" t="n"/>
-      <c r="B287" s="5" t="n"/>
-      <c r="C287" s="5" t="n"/>
-      <c r="D287" s="6" t="n"/>
-      <c r="E287" s="2" t="n"/>
-      <c r="F287" s="7" t="n"/>
-      <c r="G287" s="8" t="n"/>
-      <c r="H287" s="8" t="n"/>
-      <c r="I287" s="8" t="n"/>
-      <c r="J287" s="2" t="n"/>
-      <c r="K287" s="2" t="n"/>
-      <c r="L287" s="8" t="n"/>
-      <c r="M287" s="8" t="n"/>
-      <c r="N287" s="8" t="n"/>
-      <c r="O287" s="2" t="n"/>
-      <c r="P287" s="2" t="n"/>
-      <c r="Q287" s="8" t="n"/>
-      <c r="R287" s="8" t="n"/>
-      <c r="S287" s="8" t="n"/>
-      <c r="T287" s="2" t="n"/>
-      <c r="U287" s="2" t="n"/>
-      <c r="V287" s="8" t="n"/>
-      <c r="W287" s="8" t="n"/>
-      <c r="X287" s="8" t="n"/>
-      <c r="Y287" s="2" t="n"/>
-      <c r="Z287" s="2" t="n"/>
-      <c r="AA287" s="8" t="n"/>
-      <c r="AB287" s="8" t="n"/>
-      <c r="AC287" s="8" t="n"/>
-      <c r="AD287" s="2" t="n"/>
-      <c r="AE287" s="2" t="n">
-        <v>1110</v>
-      </c>
-      <c r="AF287" s="8" t="n">
-        <v>38.85</v>
-      </c>
-      <c r="AG287" s="8" t="n">
-        <v>11.1</v>
-      </c>
-      <c r="AH287" s="8" t="n">
-        <v>1159.95</v>
-      </c>
-      <c r="AI287" s="2" t="n"/>
-      <c r="AJ287" s="2" t="n"/>
-      <c r="AK287" s="8" t="n"/>
-      <c r="AL287" s="8" t="n"/>
-      <c r="AM287" s="8" t="n"/>
-      <c r="AN287" s="2" t="n"/>
-      <c r="AO287" s="2" t="n"/>
-      <c r="AP287" s="8" t="n"/>
-      <c r="AQ287" s="8" t="n"/>
-      <c r="AR287" s="8" t="n"/>
-      <c r="AS287" s="2" t="n"/>
-      <c r="AT287" s="2" t="n"/>
-      <c r="AU287" s="8" t="n"/>
-      <c r="AV287" s="8" t="n"/>
-      <c r="AW287" s="8" t="n"/>
-      <c r="AX287" s="2" t="n"/>
-      <c r="AY287" s="2" t="n"/>
-      <c r="AZ287" s="8" t="n"/>
-      <c r="BA287" s="8" t="n"/>
-      <c r="BB287" s="8" t="n"/>
-      <c r="BC287" s="2" t="n"/>
-      <c r="BD287" s="2" t="n"/>
-      <c r="BE287" s="8" t="n"/>
-      <c r="BF287" s="8" t="n"/>
-      <c r="BG287" s="8" t="n"/>
-      <c r="BH287" s="2" t="n"/>
-      <c r="BI287" s="2" t="n"/>
-      <c r="BJ287" s="8" t="n"/>
-      <c r="BK287" s="8" t="n"/>
-      <c r="BL287" s="8" t="n"/>
-      <c r="BM287" s="2" t="n"/>
-      <c r="BN287" s="2" t="n"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="V1:Z1"/>

</xml_diff>